<commit_message>
Placement: Deloitte Practice Set Uploaded
</commit_message>
<xml_diff>
--- a/project/MRU Java FSD Project Final.xlsx
+++ b/project/MRU Java FSD Project Final.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="140">
   <si>
     <t xml:space="preserve">University </t>
   </si>
@@ -309,145 +309,142 @@
     <t>PUSHKARINEE</t>
   </si>
   <si>
-    <t>THE NAVIGATORS</t>
+    <t>K.SAINATH DORA</t>
+  </si>
+  <si>
+    <t>K. PRANAHITHA</t>
+  </si>
+  <si>
+    <t>A. NAGA HARSHITHA</t>
+  </si>
+  <si>
+    <t>H.SARAYU CHOWHAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KUNTA BHAGEERATH </t>
+  </si>
+  <si>
+    <t>B.KARTHIK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIVA BOJJANI </t>
+  </si>
+  <si>
+    <t>G.PRASHANTH</t>
+  </si>
+  <si>
+    <t>ABHINAY DATTA</t>
+  </si>
+  <si>
+    <t>ABHISHEK PANDEY</t>
+  </si>
+  <si>
+    <t>C.SAMEEKSHA</t>
+  </si>
+  <si>
+    <t>D.TANUJA</t>
+  </si>
+  <si>
+    <t>MOKSHESHWAR REDDY</t>
+  </si>
+  <si>
+    <t>BHAGEERATH</t>
+  </si>
+  <si>
+    <t>SHIVA</t>
+  </si>
+  <si>
+    <t>CH.SATHWIKA REDDY</t>
+  </si>
+  <si>
+    <t>J.SOWJANYA REDDY</t>
+  </si>
+  <si>
+    <t>M. SANDEEPTHI CHAITRAN</t>
+  </si>
+  <si>
+    <t>R. VENKATESH</t>
+  </si>
+  <si>
+    <t>M. SHIVA KRISHNA</t>
+  </si>
+  <si>
+    <t>RAYANAPALLI POOJITHA</t>
+  </si>
+  <si>
+    <t>MD.JAVEED KHAN</t>
+  </si>
+  <si>
+    <t>M.NANDINI</t>
+  </si>
+  <si>
+    <t>G.POOJITHA</t>
+  </si>
+  <si>
+    <t>T.SWETHA</t>
+  </si>
+  <si>
+    <t>R.SUCHITRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOHAMMED ISMAIL </t>
+  </si>
+  <si>
+    <t>VAMSHI</t>
+  </si>
+  <si>
+    <t>V.MAMATHA</t>
+  </si>
+  <si>
+    <t>M.PRAVALIKA</t>
+  </si>
+  <si>
+    <t>PRAVALIKA</t>
+  </si>
+  <si>
+    <t>VANGALA HARI VIGHNESH</t>
+  </si>
+  <si>
+    <t>V.CHARAN SAI</t>
+  </si>
+  <si>
+    <t>ASINSHAIK</t>
+  </si>
+  <si>
+    <t>MOHAMMED SALAUDDIN</t>
+  </si>
+  <si>
+    <t>V.AJITH KUMAR</t>
+  </si>
+  <si>
+    <t>NITHIN MARRI</t>
+  </si>
+  <si>
+    <t>G.MANIKANTA</t>
+  </si>
+  <si>
+    <t>M.VIJAY KUMAR</t>
+  </si>
+  <si>
+    <t>VISHAL</t>
+  </si>
+  <si>
+    <t>NAIKI SAIKUMAR</t>
+  </si>
+  <si>
+    <t>M.RADHAKRISHNA</t>
+  </si>
+  <si>
+    <t>SANJAY DANIEL</t>
+  </si>
+  <si>
+    <t>2211CS0130109</t>
+  </si>
+  <si>
+    <t>2211CS030012</t>
   </si>
   <si>
     <t>DOUTHAPURAM PRANAY</t>
-  </si>
-  <si>
-    <t>K.SAINATH DORA</t>
-  </si>
-  <si>
-    <t>K. PRANAHITHA</t>
-  </si>
-  <si>
-    <t>A. NAGA HARSHITHA</t>
-  </si>
-  <si>
-    <t>H.SARAYU CHOWHAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KUNTA BHAGEERATH </t>
-  </si>
-  <si>
-    <t>B.KARTHIK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIVA BOJJANI </t>
-  </si>
-  <si>
-    <t>G.PRASHANTH</t>
-  </si>
-  <si>
-    <t>ABHINAY DATTA</t>
-  </si>
-  <si>
-    <t>ABHISHEK PANDEY</t>
-  </si>
-  <si>
-    <t>C.SAMEEKSHA</t>
-  </si>
-  <si>
-    <t>D.TANUJA</t>
-  </si>
-  <si>
-    <t>MOKSHESHWAR REDDY</t>
-  </si>
-  <si>
-    <t>BHAGEERATH</t>
-  </si>
-  <si>
-    <t>SHIVA</t>
-  </si>
-  <si>
-    <t>CH.SATHWIKA REDDY</t>
-  </si>
-  <si>
-    <t>J.SOWJANYA REDDY</t>
-  </si>
-  <si>
-    <t>M. SANDEEPTHI CHAITRAN</t>
-  </si>
-  <si>
-    <t>R. VENKATESH</t>
-  </si>
-  <si>
-    <t>M. SHIVA KRISHNA</t>
-  </si>
-  <si>
-    <t>RAYANAPALLI POOJITHA</t>
-  </si>
-  <si>
-    <t>MD.JAVEED KHAN</t>
-  </si>
-  <si>
-    <t>M.NANDINI</t>
-  </si>
-  <si>
-    <t>G.POOJITHA</t>
-  </si>
-  <si>
-    <t>T.SWETHA</t>
-  </si>
-  <si>
-    <t>R.SUCHITRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOHAMMED ISMAIL </t>
-  </si>
-  <si>
-    <t>VAMSHI</t>
-  </si>
-  <si>
-    <t>V.MAMATHA</t>
-  </si>
-  <si>
-    <t>M.PRAVALIKA</t>
-  </si>
-  <si>
-    <t>PRAVALIKA</t>
-  </si>
-  <si>
-    <t>VANGALA HARI VIGHNESH</t>
-  </si>
-  <si>
-    <t>V.CHARAN SAI</t>
-  </si>
-  <si>
-    <t>ASINSHAIK</t>
-  </si>
-  <si>
-    <t>MOHAMMED SALAUDDIN</t>
-  </si>
-  <si>
-    <t>V.AJITH KUMAR</t>
-  </si>
-  <si>
-    <t>NITHIN MARRI</t>
-  </si>
-  <si>
-    <t>G.MANIKANTA</t>
-  </si>
-  <si>
-    <t>M.VIJAY KUMAR</t>
-  </si>
-  <si>
-    <t>VISHAL</t>
-  </si>
-  <si>
-    <t>NAIKI SAIKUMAR</t>
-  </si>
-  <si>
-    <t>M.RADHAKRISHNA</t>
-  </si>
-  <si>
-    <t>SANJAY DANIEL</t>
-  </si>
-  <si>
-    <t>2211CS0130109</t>
-  </si>
-  <si>
-    <t>2211CS030012</t>
   </si>
 </sst>
 </file>
@@ -641,6 +638,180 @@
   <dxfs count="30">
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -819,180 +990,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1007,24 +1004,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:J60" headerRowDxfId="21" dataDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:J60" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:J60"/>
   <sortState ref="A2:J60">
     <sortCondition ref="A1:A60"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" name="S.no" dataDxfId="22"/>
-    <tableColumn id="2" name="University " dataDxfId="23"/>
-    <tableColumn id="3" name="Department" dataDxfId="20"/>
-    <tableColumn id="4" name="Project Title" dataDxfId="18">
+    <tableColumn id="1" name="S.no" dataDxfId="9"/>
+    <tableColumn id="2" name="University " dataDxfId="8"/>
+    <tableColumn id="3" name="Department" dataDxfId="7"/>
+    <tableColumn id="4" name="Project Title" dataDxfId="6">
       <calculatedColumnFormula>UPPER(Form_Responses1[[#This Row],[Project Title]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Application Name" dataDxfId="19"/>
-    <tableColumn id="5" name="Team Leader Name" dataDxfId="24"/>
-    <tableColumn id="6" name="Team Leader Roll No" dataDxfId="28"/>
-    <tableColumn id="7" name="Batch" dataDxfId="27"/>
-    <tableColumn id="8" name="Status" dataDxfId="26"/>
-    <tableColumn id="9" name="Remarks" dataDxfId="25"/>
+    <tableColumn id="11" name="Application Name" dataDxfId="5"/>
+    <tableColumn id="5" name="Team Leader Name" dataDxfId="4"/>
+    <tableColumn id="6" name="Team Leader Roll No" dataDxfId="3"/>
+    <tableColumn id="7" name="Batch" dataDxfId="2"/>
+    <tableColumn id="8" name="Status" dataDxfId="1"/>
+    <tableColumn id="9" name="Remarks" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1300,7 +1297,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1703,8 +1700,9 @@
         <f ca="1">UPPER(Form_Responses1[[#This Row],[Project Title]])</f>
         <v>HOBBY TRAVEL MATCHMAKER</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>94</v>
+      <c r="F14" s="5" t="str">
+        <f ca="1">UPPER(Form_Responses1[[#This Row],[Team Leader Name]])</f>
+        <v>G.SAI KAVYA</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>33</v>
@@ -1731,8 +1729,8 @@
         <f ca="1">UPPER(Form_Responses1[[#This Row],[Project Title]])</f>
         <v>VEHICLE SERVICE MANAGEMENT SYSTEM</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>95</v>
+      <c r="F15" s="8" t="s">
+        <v>139</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>34</v>
@@ -1760,7 +1758,7 @@
         <v>SKILL EXCHANGE PLATFORM</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>35</v>
@@ -1788,7 +1786,7 @@
         <v>MOVIE CLUB MANAGEMENT APP</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>36</v>
@@ -1816,7 +1814,7 @@
         <v>VIRTUAL FOOD FESTIVAL APP</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>37</v>
@@ -1844,7 +1842,7 @@
         <v>SOCIAL FITNESS CHALLENGES PLATFORM</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>39</v>
@@ -1872,7 +1870,7 @@
         <v xml:space="preserve">TODO LIST </v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>45</v>
@@ -1902,7 +1900,7 @@
         <v>AIRLINE MANAGEMENT SYSTEM</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>46</v>
@@ -1930,7 +1928,7 @@
         <v xml:space="preserve">TRAVEL JOURNAL </v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>47</v>
@@ -1958,7 +1956,7 @@
         <v>TRAVEL ITINERARY PLANNING</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>48</v>
@@ -1988,10 +1986,10 @@
         <v xml:space="preserve">JOB PORTAL </v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>75</v>
@@ -2018,7 +2016,7 @@
         <v>SUSTAINABLE LIVING PLATFORM</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>56</v>
@@ -2046,7 +2044,7 @@
         <v>FIND A WAY</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>57</v>
@@ -2074,7 +2072,7 @@
         <v>CAFÉ MANAGEMENT SYSTEM</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>58</v>
@@ -2102,7 +2100,7 @@
         <v>EMPLOYEE MANAGEMENT SYSTEM</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>61</v>
@@ -2130,7 +2128,7 @@
         <v>MUSIC STREAMING SERVICE</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>62</v>
@@ -2158,10 +2156,10 @@
         <v>ENVIRONMENTAL AWARENESS &amp; VOLUNTEER ENGAGEMENT PLATFORM</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>75</v>
@@ -2186,7 +2184,7 @@
         <v>RETIREMENT HOME MANAGEMENT</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>79</v>
@@ -2214,7 +2212,7 @@
         <v>CAMPUS PLACEMENT MANGEMENT APP</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>80</v>
@@ -2242,7 +2240,7 @@
         <v xml:space="preserve"> E-LEARNING PLATFORM WITH GAMIFICATION</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>18</v>
@@ -2270,7 +2268,7 @@
         <v>ADVENTURE PLANNER PLATFORM</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>24</v>
@@ -2298,7 +2296,7 @@
         <v>APPOINTMENT SCHEDULING SYSTEM</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>27</v>
@@ -2328,7 +2326,7 @@
         <v>BOOKSWAP</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>38</v>
@@ -2356,7 +2354,7 @@
         <v>CONTACT BOOK</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>40</v>
@@ -2386,7 +2384,7 @@
         <v>REAL-TIME QUIZ &amp; HACKATHON PLATFORM:</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>42</v>
@@ -2442,7 +2440,7 @@
         <v>ONLINE BOOKSTORE</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>51</v>
@@ -2472,7 +2470,7 @@
         <v xml:space="preserve">TASK MANAGER </v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>52</v>
@@ -2502,7 +2500,7 @@
         <v>REAL-TIME MULTIPLAYER CHESS GAME</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>53</v>
@@ -2530,7 +2528,7 @@
         <v xml:space="preserve">USER MANAGEMENT APPLICATION </v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>54</v>
@@ -2560,7 +2558,7 @@
         <v>PG MADE EAZY</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G44" s="21" t="s">
         <v>59</v>
@@ -2588,7 +2586,7 @@
         <v>WOMEN COMMUNITY FORUM</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G45" s="21" t="s">
         <v>60</v>
@@ -2616,7 +2614,7 @@
         <v>SMART PARKING FINDER PLATFORM</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G46" s="21" t="s">
         <v>81</v>
@@ -2644,7 +2642,7 @@
         <v>FASHION SUSTAINABILITY HUB</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G47" s="21" t="s">
         <v>82</v>
@@ -2672,7 +2670,7 @@
         <v>ECHOBEAT</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G48" s="21" t="s">
         <v>83</v>
@@ -2702,7 +2700,7 @@
         <v>SMART KNOWLEDGE HUB</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G49" s="21" t="s">
         <v>63</v>
@@ -2730,7 +2728,7 @@
         <v>PEER-TO-PEER CAR RENTAL PLATFORM WITH DELIVERY &amp; PICKUP SERVICE</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G50" s="21" t="s">
         <v>64</v>
@@ -2758,7 +2756,7 @@
         <v>FASHION E-COMMERCE WITH AI</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G51" s="21" t="s">
         <v>84</v>
@@ -2786,7 +2784,7 @@
         <v>SMART SOLAR MANAGEMENT SYSTEM</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G52" s="21" t="s">
         <v>85</v>
@@ -2799,7 +2797,7 @@
       </c>
       <c r="J52" s="5"/>
     </row>
-    <row r="53" spans="1:12" ht="43.2">
+    <row r="53" spans="1:12" ht="31.2">
       <c r="A53" s="9">
         <v>52</v>
       </c>
@@ -2814,7 +2812,7 @@
         <v>HEALTH AND WELLNESS MARKETPLACE WITH PERSONALIZED FITNESS &amp; NUTRITION PLATFORM</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G53" s="21" t="s">
         <v>65</v>
@@ -2842,7 +2840,7 @@
         <v>FITLETICS - A COMPLETE ATHLETIC APP</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G54" s="21" t="s">
         <v>66</v>
@@ -2870,7 +2868,7 @@
         <v>CAR POOLING PLATFORM</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G55" s="21" t="s">
         <v>67</v>
@@ -2926,7 +2924,7 @@
         <v>RENTAL MANAGEMENT &amp; COMMUNITY HOUSING HUB</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G57" s="21" t="s">
         <v>70</v>
@@ -2954,7 +2952,7 @@
         <v>GRANDMA’S SWEETS AND PICKLES E-COMMERCE PLATFORM</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G58" s="21" t="s">
         <v>86</v>
@@ -2982,7 +2980,7 @@
         <v>PLAN IT NOW</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G59" s="21" t="s">
         <v>71</v>
@@ -3012,7 +3010,7 @@
         <v>STARTUP NEWBIES</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G60" s="21" t="s">
         <v>72</v>
@@ -3755,58 +3753,58 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I61:I1048576 I1">
-    <cfRule type="containsText" dxfId="17" priority="21" operator="containsText" text="Pending">
+    <cfRule type="containsText" dxfId="29" priority="21" operator="containsText" text="Pending">
       <formula>NOT(ISERROR(SEARCH("Pending",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="22" operator="containsText" text="Accepted">
+    <cfRule type="containsText" dxfId="28" priority="22" operator="containsText" text="Accepted">
       <formula>NOT(ISERROR(SEARCH("Accepted",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="23" operator="containsText" text="Rejected">
+    <cfRule type="containsText" dxfId="27" priority="23" operator="containsText" text="Rejected">
       <formula>NOT(ISERROR(SEARCH("Rejected",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G61 G1 G153:G1048576">
-    <cfRule type="duplicateValues" dxfId="14" priority="16"/>
-    <cfRule type="duplicateValues" dxfId="13" priority="20"/>
-    <cfRule type="duplicateValues" dxfId="12" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F61:F1048576 F1">
-    <cfRule type="duplicateValues" dxfId="11" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="duplicateValues" dxfId="10" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="Rejected">
+    <cfRule type="containsText" dxfId="21" priority="13" operator="containsText" text="Rejected">
       <formula>NOT(ISERROR(SEARCH("Rejected",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="14" operator="containsText" text="Accepted">
+    <cfRule type="containsText" dxfId="20" priority="14" operator="containsText" text="Accepted">
       <formula>NOT(ISERROR(SEARCH("Accepted",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G62">
-    <cfRule type="duplicateValues" dxfId="7" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G62 G153:G1048576">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G70">
-    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G120">
-    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G126 G147:G148 G139 G68">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G151 G149 G127 G144:G146 G140:G142 G129:G138 G121:G125 G72:G119 G63:G67 G69">
-    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G152 G150 G128 G143 G71">
-    <cfRule type="duplicateValues" dxfId="1" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
React Basics: form handling updated
</commit_message>
<xml_diff>
--- a/project/MRU Java FSD Project Final.xlsx
+++ b/project/MRU Java FSD Project Final.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="197">
   <si>
     <t xml:space="preserve">University </t>
   </si>
@@ -176,9 +176,6 @@
     <t>2211CS030119</t>
   </si>
   <si>
-    <t>Lack of innovative ideas</t>
-  </si>
-  <si>
     <t>2211CS030041</t>
   </si>
   <si>
@@ -350,18 +347,12 @@
     <t>M.NANDINI</t>
   </si>
   <si>
-    <t>G.POOJITHA</t>
-  </si>
-  <si>
     <t>T.SWETHA</t>
   </si>
   <si>
     <t>R.SUCHITRA</t>
   </si>
   <si>
-    <t xml:space="preserve">MOHAMMED ISMAIL </t>
-  </si>
-  <si>
     <t>VAMSHI</t>
   </si>
   <si>
@@ -476,9 +467,6 @@
     <t xml:space="preserve">TRAVEL JOURNAL </t>
   </si>
   <si>
-    <t>TRAVEL ITINERARY PLANNING</t>
-  </si>
-  <si>
     <t>SUSTAINABLE LIVING PLATFORM</t>
   </si>
   <si>
@@ -509,27 +497,18 @@
     <t>BOOKSWAP</t>
   </si>
   <si>
-    <t>CONTACT BOOK</t>
-  </si>
-  <si>
     <t>REAL-TIME QUIZ &amp; HACKATHON PLATFORM:</t>
   </si>
   <si>
     <t>INVENTORY MANAGEMENT</t>
   </si>
   <si>
-    <t>ONLINE BOOKSTORE</t>
-  </si>
-  <si>
     <t xml:space="preserve">TASK MANAGER </t>
   </si>
   <si>
     <t>REAL-TIME MULTIPLAYER CHESS GAME</t>
   </si>
   <si>
-    <t xml:space="preserve">USER MANAGEMENT APPLICATION </t>
-  </si>
-  <si>
     <t>PG MADE EAZY</t>
   </si>
   <si>
@@ -615,6 +594,27 @@
   </si>
   <si>
     <t>P.SANJEEVA RAO</t>
+  </si>
+  <si>
+    <t>2211CS030065</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1YVkDNKSmijvKI5GUkTXSX0mpqFa4icJX</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1SQ_HzKJn8f1aD27_ij_KwRAQZBePkWVF</t>
+  </si>
+  <si>
+    <t>G.SACHIN REDDY</t>
+  </si>
+  <si>
+    <t>SMART WASTE MANAGEMENT SYSTEM</t>
+  </si>
+  <si>
+    <t>NEED TO DECIDE</t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
 </sst>
 </file>
@@ -624,7 +624,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -677,6 +677,14 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -697,7 +705,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -759,12 +767,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -856,12 +878,424 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="31">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1042,418 +1476,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1468,19 +1490,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:J62" headerRowDxfId="34" dataDxfId="33">
-  <autoFilter ref="A1:J62"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:J60" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J60"/>
+  <sortState ref="A2:J60">
+    <sortCondition ref="A1:A60"/>
+  </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" name="S.no" dataDxfId="32"/>
-    <tableColumn id="2" name="University " dataDxfId="31"/>
-    <tableColumn id="3" name="Department" dataDxfId="23"/>
-    <tableColumn id="4" name="Project Title" dataDxfId="30"/>
-    <tableColumn id="11" name="Application Name" dataDxfId="29"/>
-    <tableColumn id="5" name="Team Leader Name" dataDxfId="28"/>
-    <tableColumn id="6" name="Team Leader Roll No" dataDxfId="24"/>
-    <tableColumn id="7" name="Batch" dataDxfId="27"/>
-    <tableColumn id="8" name="Status" dataDxfId="26"/>
-    <tableColumn id="9" name="Remarks" dataDxfId="25"/>
+    <tableColumn id="1" name="S.no" dataDxfId="9"/>
+    <tableColumn id="2" name="University " dataDxfId="8"/>
+    <tableColumn id="3" name="Department" dataDxfId="7"/>
+    <tableColumn id="4" name="Project Title" dataDxfId="6"/>
+    <tableColumn id="11" name="Application Name" dataDxfId="5"/>
+    <tableColumn id="5" name="Team Leader Name" dataDxfId="4"/>
+    <tableColumn id="6" name="Team Leader Roll No" dataDxfId="3"/>
+    <tableColumn id="7" name="Batch" dataDxfId="2"/>
+    <tableColumn id="8" name="Status" dataDxfId="1"/>
+    <tableColumn id="9" name="Remarks" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1752,11 +1777,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L149"/>
+  <dimension ref="A1:L145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F65" sqref="F65"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1777,7 +1802,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -1789,7 +1814,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>3</v>
@@ -1798,7 +1823,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>5</v>
@@ -1818,7 +1843,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E2" s="17"/>
       <c r="F2" s="15" t="s">
@@ -1828,7 +1853,7 @@
         <v>10</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I2" s="15" t="s">
         <v>13</v>
@@ -1846,17 +1871,17 @@
         <v>8</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E3" s="17"/>
       <c r="F3" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G3" s="18" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I3" s="15" t="s">
         <v>13</v>
@@ -1874,7 +1899,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E4" s="17"/>
       <c r="F4" s="15" t="s">
@@ -1884,7 +1909,7 @@
         <v>15</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I4" s="15" t="s">
         <v>13</v>
@@ -1902,7 +1927,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="15" t="s">
@@ -1912,7 +1937,7 @@
         <v>17</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I5" s="15" t="s">
         <v>13</v>
@@ -1930,17 +1955,17 @@
         <v>8</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E6" s="17"/>
       <c r="F6" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G6" s="18" t="s">
         <v>19</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I6" s="15" t="s">
         <v>13</v>
@@ -1958,17 +1983,17 @@
         <v>8</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E7" s="17"/>
       <c r="F7" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G7" s="18" t="s">
         <v>20</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I7" s="15" t="s">
         <v>13</v>
@@ -1986,17 +2011,17 @@
         <v>8</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G8" s="18" t="s">
         <v>21</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I8" s="15" t="s">
         <v>13</v>
@@ -2014,7 +2039,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E9" s="17"/>
       <c r="F9" s="15" t="s">
@@ -2024,7 +2049,7 @@
         <v>23</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I9" s="15" t="s">
         <v>13</v>
@@ -2042,17 +2067,17 @@
         <v>8</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E10" s="17"/>
       <c r="F10" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G10" s="18" t="s">
         <v>25</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I10" s="15" t="s">
         <v>13</v>
@@ -2070,17 +2095,17 @@
         <v>8</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E11" s="17"/>
       <c r="F11" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G11" s="18" t="s">
         <v>26</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I11" s="15" t="s">
         <v>13</v>
@@ -2098,7 +2123,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="15" t="s">
@@ -2108,7 +2133,7 @@
         <v>29</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I12" s="15" t="s">
         <v>13</v>
@@ -2126,7 +2151,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="20" t="str">
@@ -2137,7 +2162,7 @@
         <v>30</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I13" s="15" t="s">
         <v>13</v>
@@ -2155,17 +2180,17 @@
         <v>8</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="19" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G14" s="18" t="s">
         <v>31</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I14" s="15" t="s">
         <v>13</v>
@@ -2183,17 +2208,17 @@
         <v>8</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E15" s="17"/>
       <c r="F15" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G15" s="18" t="s">
         <v>32</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I15" s="15" t="s">
         <v>13</v>
@@ -2211,17 +2236,17 @@
         <v>8</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E16" s="17"/>
       <c r="F16" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G16" s="18" t="s">
         <v>33</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I16" s="15" t="s">
         <v>13</v>
@@ -2239,24 +2264,24 @@
         <v>8</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E17" s="17"/>
       <c r="F17" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G17" s="18" t="s">
         <v>34</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I17" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J17" s="20"/>
     </row>
-    <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14">
         <v>18</v>
       </c>
@@ -2267,17 +2292,17 @@
         <v>8</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G18" s="18" t="s">
         <v>36</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I18" s="15" t="s">
         <v>13</v>
@@ -2295,17 +2320,17 @@
         <v>8</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G19" s="18" t="s">
         <v>42</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I19" s="15" t="s">
         <v>13</v>
@@ -2323,17 +2348,17 @@
         <v>8</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G20" s="18" t="s">
         <v>43</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I20" s="15" t="s">
         <v>13</v>
@@ -2342,7 +2367,7 @@
     </row>
     <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>7</v>
@@ -2351,28 +2376,26 @@
         <v>8</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>150</v>
+        <v>178</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="15" t="s">
         <v>93</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>44</v>
+        <v>125</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J21" s="21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="J21" s="22"/>
+    </row>
+    <row r="22" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>7</v>
@@ -2381,26 +2404,28 @@
         <v>8</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="E22" s="17"/>
+        <v>147</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>180</v>
+      </c>
       <c r="F22" s="15" t="s">
         <v>94</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>128</v>
+        <v>179</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I22" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="J22" s="22"/>
+      <c r="J22" s="20"/>
     </row>
     <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>7</v>
@@ -2409,19 +2434,17 @@
         <v>8</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>187</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="E23" s="17"/>
       <c r="F23" s="15" t="s">
         <v>95</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>186</v>
+        <v>50</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I23" s="15" t="s">
         <v>13</v>
@@ -2430,7 +2453,7 @@
     </row>
     <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B24" s="15" t="s">
         <v>7</v>
@@ -2439,7 +2462,7 @@
         <v>8</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="15" t="s">
@@ -2449,7 +2472,7 @@
         <v>51</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I24" s="15" t="s">
         <v>13</v>
@@ -2458,7 +2481,7 @@
     </row>
     <row r="25" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="14">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B25" s="15" t="s">
         <v>7</v>
@@ -2467,17 +2490,17 @@
         <v>8</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="15" t="s">
         <v>97</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I25" s="15" t="s">
         <v>13</v>
@@ -2486,7 +2509,7 @@
     </row>
     <row r="26" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="14">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>7</v>
@@ -2495,7 +2518,7 @@
         <v>8</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="15" t="s">
@@ -2505,7 +2528,7 @@
         <v>55</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I26" s="15" t="s">
         <v>13</v>
@@ -2514,7 +2537,7 @@
     </row>
     <row r="27" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="14">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>7</v>
@@ -2523,17 +2546,17 @@
         <v>8</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="15" t="s">
         <v>99</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I27" s="15" t="s">
         <v>13</v>
@@ -2542,7 +2565,7 @@
     </row>
     <row r="28" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="14">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>7</v>
@@ -2551,7 +2574,7 @@
         <v>8</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="15" t="s">
@@ -2561,7 +2584,7 @@
         <v>73</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I28" s="15" t="s">
         <v>13</v>
@@ -2570,7 +2593,7 @@
     </row>
     <row r="29" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="14">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>7</v>
@@ -2579,14 +2602,14 @@
         <v>8</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="15" t="s">
         <v>101</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>74</v>
+        <v>18</v>
       </c>
       <c r="H29" s="15" t="s">
         <v>69</v>
@@ -2598,7 +2621,7 @@
     </row>
     <row r="30" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="14">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B30" s="15" t="s">
         <v>7</v>
@@ -2607,17 +2630,17 @@
         <v>8</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="15" t="s">
         <v>102</v>
       </c>
       <c r="G30" s="18" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I30" s="15" t="s">
         <v>13</v>
@@ -2626,7 +2649,7 @@
     </row>
     <row r="31" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="14">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B31" s="15" t="s">
         <v>7</v>
@@ -2635,26 +2658,26 @@
         <v>8</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
       <c r="E31" s="17"/>
       <c r="F31" s="15" t="s">
         <v>103</v>
       </c>
       <c r="G31" s="18" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I31" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="J31" s="20"/>
+      <c r="J31" s="22"/>
     </row>
     <row r="32" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="14">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B32" s="15" t="s">
         <v>7</v>
@@ -2663,26 +2686,26 @@
         <v>8</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="E32" s="17"/>
       <c r="F32" s="15" t="s">
         <v>104</v>
       </c>
       <c r="G32" s="18" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I32" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="J32" s="22"/>
+      <c r="J32" s="20"/>
     </row>
     <row r="33" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="14">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B33" s="15" t="s">
         <v>7</v>
@@ -2691,17 +2714,17 @@
         <v>8</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E33" s="17"/>
       <c r="F33" s="15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G33" s="18" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I33" s="15" t="s">
         <v>13</v>
@@ -2710,7 +2733,7 @@
     </row>
     <row r="34" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="14">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B34" s="15" t="s">
         <v>7</v>
@@ -2719,28 +2742,26 @@
         <v>8</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E34" s="17"/>
       <c r="F34" s="15" t="s">
-        <v>106</v>
+        <v>40</v>
       </c>
       <c r="G34" s="18" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I34" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J34" s="21" t="s">
-        <v>38</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="J34" s="20"/>
     </row>
     <row r="35" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="14">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B35" s="15" t="s">
         <v>7</v>
@@ -2749,26 +2770,28 @@
         <v>8</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E35" s="17"/>
       <c r="F35" s="15" t="s">
         <v>107</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I35" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J35" s="20"/>
+        <v>11</v>
+      </c>
+      <c r="J35" s="21" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="36" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="14">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B36" s="15" t="s">
         <v>7</v>
@@ -2777,17 +2800,17 @@
         <v>8</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E36" s="17"/>
       <c r="F36" s="15" t="s">
-        <v>40</v>
+        <v>108</v>
       </c>
       <c r="G36" s="18" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I36" s="15" t="s">
         <v>13</v>
@@ -2796,7 +2819,7 @@
     </row>
     <row r="37" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="14">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B37" s="15" t="s">
         <v>7</v>
@@ -2805,28 +2828,26 @@
         <v>8</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E37" s="17"/>
       <c r="F37" s="15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G37" s="18" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="H37" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J37" s="21" t="s">
-        <v>45</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="J37" s="20"/>
     </row>
     <row r="38" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="14">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B38" s="15" t="s">
         <v>7</v>
@@ -2835,28 +2856,26 @@
         <v>8</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E38" s="17"/>
       <c r="F38" s="15" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G38" s="18" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I38" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J38" s="21" t="s">
-        <v>45</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="J38" s="20"/>
     </row>
     <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="14">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B39" s="15" t="s">
         <v>7</v>
@@ -2865,17 +2884,17 @@
         <v>8</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E39" s="17"/>
       <c r="F39" s="15" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G39" s="18" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I39" s="15" t="s">
         <v>13</v>
@@ -2884,7 +2903,7 @@
     </row>
     <row r="40" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="14">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B40" s="15" t="s">
         <v>7</v>
@@ -2893,28 +2912,26 @@
         <v>8</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E40" s="17"/>
       <c r="F40" s="15" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G40" s="18" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I40" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J40" s="21" t="s">
-        <v>50</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="J40" s="20"/>
     </row>
     <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="14">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B41" s="15" t="s">
         <v>7</v>
@@ -2923,26 +2940,28 @@
         <v>8</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E41" s="17"/>
       <c r="F41" s="15" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G41" s="18" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I41" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J41" s="20"/>
+        <v>11</v>
+      </c>
+      <c r="J41" s="21" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="42" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="14">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B42" s="15" t="s">
         <v>7</v>
@@ -2951,17 +2970,17 @@
         <v>8</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E42" s="17"/>
       <c r="F42" s="15" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G42" s="18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H42" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I42" s="15" t="s">
         <v>13</v>
@@ -2970,7 +2989,7 @@
     </row>
     <row r="43" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="14">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B43" s="15" t="s">
         <v>7</v>
@@ -2979,17 +2998,17 @@
         <v>8</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E43" s="17"/>
       <c r="F43" s="15" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G43" s="18" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="H43" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I43" s="15" t="s">
         <v>13</v>
@@ -2998,7 +3017,7 @@
     </row>
     <row r="44" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="14">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B44" s="15" t="s">
         <v>7</v>
@@ -3007,17 +3026,17 @@
         <v>8</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="E44" s="17"/>
       <c r="F44" s="15" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G44" s="18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H44" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I44" s="15" t="s">
         <v>13</v>
@@ -3026,7 +3045,7 @@
     </row>
     <row r="45" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="14">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B45" s="15" t="s">
         <v>7</v>
@@ -3035,28 +3054,26 @@
         <v>8</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E45" s="17"/>
       <c r="F45" s="15" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G45" s="18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H45" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I45" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J45" s="21" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="J45" s="20"/>
+    </row>
+    <row r="46" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A46" s="14">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B46" s="15" t="s">
         <v>7</v>
@@ -3065,17 +3082,17 @@
         <v>8</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E46" s="17"/>
       <c r="F46" s="15" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G46" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H46" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I46" s="15" t="s">
         <v>13</v>
@@ -3084,7 +3101,7 @@
     </row>
     <row r="47" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="14">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B47" s="15" t="s">
         <v>7</v>
@@ -3093,17 +3110,17 @@
         <v>8</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E47" s="17"/>
       <c r="F47" s="15" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G47" s="18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H47" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I47" s="15" t="s">
         <v>13</v>
@@ -3112,7 +3129,7 @@
     </row>
     <row r="48" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="14">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B48" s="15" t="s">
         <v>7</v>
@@ -3121,17 +3138,17 @@
         <v>8</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="E48" s="17"/>
       <c r="F48" s="15" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G48" s="18" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="H48" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I48" s="15" t="s">
         <v>13</v>
@@ -3140,7 +3157,7 @@
     </row>
     <row r="49" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="14">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B49" s="15" t="s">
         <v>7</v>
@@ -3149,26 +3166,26 @@
         <v>8</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E49" s="17"/>
       <c r="F49" s="15" t="s">
-        <v>120</v>
+        <v>61</v>
       </c>
       <c r="G49" s="18" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I49" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="20"/>
     </row>
-    <row r="50" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="14">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B50" s="15" t="s">
         <v>7</v>
@@ -3177,17 +3194,17 @@
         <v>8</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E50" s="17"/>
       <c r="F50" s="15" t="s">
         <v>121</v>
       </c>
       <c r="G50" s="18" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="H50" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I50" s="15" t="s">
         <v>13</v>
@@ -3196,7 +3213,7 @@
     </row>
     <row r="51" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="14">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B51" s="15" t="s">
         <v>7</v>
@@ -3205,17 +3222,17 @@
         <v>8</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E51" s="17"/>
       <c r="F51" s="15" t="s">
         <v>122</v>
       </c>
       <c r="G51" s="18" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="H51" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I51" s="15" t="s">
         <v>13</v>
@@ -3224,7 +3241,7 @@
     </row>
     <row r="52" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="14">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B52" s="15" t="s">
         <v>7</v>
@@ -3232,169 +3249,177 @@
       <c r="C52" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D52" s="16" t="s">
-        <v>178</v>
+      <c r="D52" s="20" t="s">
+        <v>175</v>
       </c>
       <c r="E52" s="17"/>
       <c r="F52" s="15" t="s">
         <v>123</v>
       </c>
       <c r="G52" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="H52" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="I52" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J52" s="21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="14">
+        <v>59</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="E53" s="19"/>
+      <c r="F53" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="G53" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="H53" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="I53" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J53" s="20"/>
+    </row>
+    <row r="54" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="24">
+        <v>60</v>
+      </c>
+      <c r="B54" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="E54" s="26"/>
+      <c r="F54" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G54" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="H54" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="I54" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J54" s="20"/>
+    </row>
+    <row r="55" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="24">
         <v>61</v>
       </c>
-      <c r="H52" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I52" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J52" s="20"/>
-    </row>
-    <row r="53" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="14">
-        <v>55</v>
-      </c>
-      <c r="B53" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D53" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="E53" s="17"/>
-      <c r="F53" s="15" t="s">
+      <c r="B55" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="E55" s="26"/>
+      <c r="F55" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G55" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="H55" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="I55" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J55" s="20"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="5"/>
+    </row>
+    <row r="56" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="24">
         <v>62</v>
       </c>
-      <c r="G53" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="H53" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I53" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J53" s="20"/>
-    </row>
-    <row r="54" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="14">
-        <v>56</v>
-      </c>
-      <c r="B54" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C54" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D54" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="E54" s="17"/>
-      <c r="F54" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="G54" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="H54" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I54" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J54" s="20"/>
-    </row>
-    <row r="55" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="14">
-        <v>57</v>
-      </c>
-      <c r="B55" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D55" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="E55" s="17"/>
-      <c r="F55" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="G55" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="H55" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I55" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J55" s="20"/>
-    </row>
-    <row r="56" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="14">
-        <v>58</v>
-      </c>
-      <c r="B56" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D56" s="20" t="s">
+      <c r="B56" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" s="31" t="s">
         <v>182</v>
       </c>
-      <c r="E56" s="17"/>
-      <c r="F56" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="G56" s="18" t="s">
-        <v>65</v>
+      <c r="E56" s="26"/>
+      <c r="F56" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="G56" s="28" t="s">
+        <v>46</v>
       </c>
       <c r="H56" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I56" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="J56" s="21" t="s">
-        <v>67</v>
-      </c>
+      <c r="J56" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="K56" s="5"/>
+      <c r="L56" s="5"/>
     </row>
     <row r="57" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="14">
-        <v>59</v>
-      </c>
-      <c r="B57" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C57" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D57" s="20" t="s">
+      <c r="A57" s="24">
+        <v>63</v>
+      </c>
+      <c r="B57" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="E57" s="26"/>
+      <c r="F57" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="G57" s="28" t="s">
         <v>183</v>
       </c>
-      <c r="E57" s="19"/>
-      <c r="F57" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="G57" s="18" t="s">
-        <v>66</v>
-      </c>
       <c r="H57" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I57" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J57" s="20"/>
+      <c r="K57" s="5"/>
+      <c r="L57" s="5"/>
     </row>
     <row r="58" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="24">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B58" s="25" t="s">
         <v>7</v>
@@ -3402,27 +3427,31 @@
       <c r="C58" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D58" s="25" t="s">
-        <v>192</v>
+      <c r="D58" s="31" t="s">
+        <v>184</v>
       </c>
       <c r="E58" s="26"/>
       <c r="F58" s="25" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="G58" s="28" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="H58" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I58" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J58" s="20"/>
-    </row>
-    <row r="59" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="J58" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="K58" s="5"/>
+      <c r="L58" s="5"/>
+    </row>
+    <row r="59" spans="1:12" s="36" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="24">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B59" s="25" t="s">
         <v>7</v>
@@ -3430,117 +3459,73 @@
       <c r="C59" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D59" s="25" t="s">
-        <v>193</v>
+      <c r="D59" s="33" t="s">
+        <v>194</v>
       </c>
       <c r="E59" s="26"/>
       <c r="F59" s="25" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="G59" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="H59" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I59" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J59" s="20"/>
-      <c r="K59" s="5"/>
-      <c r="L59" s="5"/>
-    </row>
-    <row r="60" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+      <c r="H59" s="34" t="s">
+        <v>191</v>
+      </c>
+      <c r="I59" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="J59" s="31"/>
+      <c r="K59" s="35"/>
+      <c r="L59" s="35"/>
+    </row>
+    <row r="60" spans="1:12" s="36" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="24">
-        <v>62</v>
-      </c>
-      <c r="B60" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C60" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D60" s="31" t="s">
-        <v>189</v>
+        <v>66</v>
+      </c>
+      <c r="B60" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" s="39" t="s">
+        <v>195</v>
       </c>
       <c r="E60" s="26"/>
       <c r="F60" s="25" t="s">
-        <v>195</v>
-      </c>
-      <c r="G60" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="H60" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I60" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J60" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="K60" s="5"/>
-      <c r="L60" s="5"/>
-    </row>
-    <row r="61" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="24">
-        <v>63</v>
-      </c>
-      <c r="B61" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C61" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D61" s="31" t="s">
-        <v>194</v>
-      </c>
-      <c r="E61" s="26"/>
-      <c r="F61" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="G60" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="H60" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="I60" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="G61" s="28" t="s">
-        <v>190</v>
-      </c>
-      <c r="H61" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I61" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J61" s="20"/>
-      <c r="K61" s="5"/>
-      <c r="L61" s="5"/>
-    </row>
-    <row r="62" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="24">
-        <v>64</v>
-      </c>
-      <c r="B62" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C62" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D62" s="31" t="s">
-        <v>191</v>
-      </c>
-      <c r="E62" s="26"/>
-      <c r="F62" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="G62" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="H62" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I62" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J62" s="23" t="s">
-        <v>67</v>
-      </c>
+      <c r="J60" s="41"/>
+      <c r="K60" s="35"/>
+      <c r="L60" s="35"/>
+    </row>
+    <row r="61" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="42"/>
+      <c r="C61" s="43"/>
+      <c r="D61" s="44"/>
+      <c r="E61" s="45"/>
+      <c r="G61" s="46"/>
+      <c r="H61" s="35"/>
+      <c r="I61" s="35"/>
+      <c r="J61" s="47"/>
+      <c r="K61" s="35"/>
+      <c r="L61" s="35"/>
+    </row>
+    <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G62" s="29"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="6"/>
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
     </row>
@@ -4208,97 +4193,72 @@
       <c r="K145" s="5"/>
       <c r="L145" s="5"/>
     </row>
-    <row r="146" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G146" s="29"/>
-      <c r="H146" s="5"/>
-      <c r="I146" s="5"/>
-      <c r="J146" s="6"/>
-      <c r="K146" s="5"/>
-      <c r="L146" s="5"/>
-    </row>
-    <row r="147" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G147" s="29"/>
-      <c r="H147" s="5"/>
-      <c r="I147" s="5"/>
-      <c r="J147" s="6"/>
-      <c r="K147" s="5"/>
-      <c r="L147" s="5"/>
-    </row>
-    <row r="148" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G148" s="29"/>
-      <c r="H148" s="5"/>
-      <c r="I148" s="5"/>
-      <c r="J148" s="6"/>
-      <c r="K148" s="5"/>
-      <c r="L148" s="5"/>
-    </row>
-    <row r="149" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G149" s="29"/>
-      <c r="H149" s="5"/>
-      <c r="I149" s="5"/>
-      <c r="J149" s="6"/>
-      <c r="K149" s="5"/>
-      <c r="L149" s="5"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="I1 I58:I1048576">
-    <cfRule type="containsText" dxfId="17" priority="22" operator="containsText" text="Pending">
+  <conditionalFormatting sqref="I1 I54:I1048576">
+    <cfRule type="containsText" dxfId="30" priority="23" operator="containsText" text="Pending">
       <formula>NOT(ISERROR(SEARCH("Pending",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="23" operator="containsText" text="Accepted">
+    <cfRule type="containsText" dxfId="29" priority="24" operator="containsText" text="Accepted">
       <formula>NOT(ISERROR(SEARCH("Accepted",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="24" operator="containsText" text="Rejected">
+    <cfRule type="containsText" dxfId="28" priority="25" operator="containsText" text="Rejected">
       <formula>NOT(ISERROR(SEARCH("Rejected",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1 G150:G1048576">
-    <cfRule type="duplicateValues" dxfId="14" priority="17"/>
-    <cfRule type="duplicateValues" dxfId="13" priority="21"/>
-    <cfRule type="duplicateValues" dxfId="12" priority="25"/>
+  <conditionalFormatting sqref="G146:G1048576 G1">
+    <cfRule type="duplicateValues" dxfId="27" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="26"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F63:F1048576 F1">
-    <cfRule type="duplicateValues" dxfId="11" priority="16"/>
+  <conditionalFormatting sqref="F61:F1048576 F1">
+    <cfRule type="duplicateValues" dxfId="24" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="duplicateValues" dxfId="10" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="containsText" dxfId="9" priority="14" operator="containsText" text="Rejected">
+    <cfRule type="containsText" dxfId="22" priority="15" operator="containsText" text="Rejected">
       <formula>NOT(ISERROR(SEARCH("Rejected",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="15" operator="containsText" text="Accepted">
+    <cfRule type="containsText" dxfId="21" priority="16" operator="containsText" text="Accepted">
       <formula>NOT(ISERROR(SEARCH("Accepted",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G150:G1048576 G1:G57">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+  <conditionalFormatting sqref="G146:G1048576 G1:G53">
+    <cfRule type="duplicateValues" dxfId="20" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G67">
-    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
+  <conditionalFormatting sqref="G63">
+    <cfRule type="duplicateValues" dxfId="19" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G117">
-    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
+  <conditionalFormatting sqref="G113">
+    <cfRule type="duplicateValues" dxfId="18" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G123 G144:G145 G136 G65">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  <conditionalFormatting sqref="G119 G140:G141 G132 G61">
+    <cfRule type="duplicateValues" dxfId="17" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G148 G146 G124 G141:G143 G137:G139 G126:G135 G118:G122 G69:G116 G63:G64 G66">
-    <cfRule type="duplicateValues" dxfId="3" priority="7"/>
+  <conditionalFormatting sqref="G144 G142 G120 G137:G139 G133:G135 G122:G131 G114:G118 G65:G112 G62">
+    <cfRule type="duplicateValues" dxfId="16" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G149 G147 G125 G140 G68">
-    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
+  <conditionalFormatting sqref="G145 G143 G121 G136 G64">
+    <cfRule type="duplicateValues" dxfId="15" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G57 G63:G1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  <conditionalFormatting sqref="G61:G1048576 G1:G53">
+    <cfRule type="duplicateValues" dxfId="14" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D63:D1048576 D1">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="D61:D1048576 D1">
+    <cfRule type="duplicateValues" dxfId="13" priority="2"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="H59" r:id="rId1"/>
+    <hyperlink ref="H60" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
till form handling reset
</commit_message>
<xml_diff>
--- a/project/MRU Java FSD Project Final.xlsx
+++ b/project/MRU Java FSD Project Final.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="197">
   <si>
     <t xml:space="preserve">University </t>
   </si>
@@ -176,6 +176,9 @@
     <t>2211CS030119</t>
   </si>
   <si>
+    <t>Lack of innovative ideas</t>
+  </si>
+  <si>
     <t>2211CS030041</t>
   </si>
   <si>
@@ -347,12 +350,18 @@
     <t>M.NANDINI</t>
   </si>
   <si>
+    <t>G.POOJITHA</t>
+  </si>
+  <si>
     <t>T.SWETHA</t>
   </si>
   <si>
     <t>R.SUCHITRA</t>
   </si>
   <si>
+    <t xml:space="preserve">MOHAMMED ISMAIL </t>
+  </si>
+  <si>
     <t>VAMSHI</t>
   </si>
   <si>
@@ -467,6 +476,9 @@
     <t xml:space="preserve">TRAVEL JOURNAL </t>
   </si>
   <si>
+    <t>TRAVEL ITINERARY PLANNING</t>
+  </si>
+  <si>
     <t>SUSTAINABLE LIVING PLATFORM</t>
   </si>
   <si>
@@ -497,18 +509,27 @@
     <t>BOOKSWAP</t>
   </si>
   <si>
+    <t>CONTACT BOOK</t>
+  </si>
+  <si>
     <t>REAL-TIME QUIZ &amp; HACKATHON PLATFORM:</t>
   </si>
   <si>
     <t>INVENTORY MANAGEMENT</t>
   </si>
   <si>
+    <t>ONLINE BOOKSTORE</t>
+  </si>
+  <si>
     <t xml:space="preserve">TASK MANAGER </t>
   </si>
   <si>
     <t>REAL-TIME MULTIPLAYER CHESS GAME</t>
   </si>
   <si>
+    <t xml:space="preserve">USER MANAGEMENT APPLICATION </t>
+  </si>
+  <si>
     <t>PG MADE EAZY</t>
   </si>
   <si>
@@ -594,27 +615,6 @@
   </si>
   <si>
     <t>P.SANJEEVA RAO</t>
-  </si>
-  <si>
-    <t>2211CS030065</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/open?id=1YVkDNKSmijvKI5GUkTXSX0mpqFa4icJX</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/open?id=1SQ_HzKJn8f1aD27_ij_KwRAQZBePkWVF</t>
-  </si>
-  <si>
-    <t>G.SACHIN REDDY</t>
-  </si>
-  <si>
-    <t>SMART WASTE MANAGEMENT SYSTEM</t>
-  </si>
-  <si>
-    <t>NEED TO DECIDE</t>
-  </si>
-  <si>
-    <t>Pending</t>
   </si>
 </sst>
 </file>
@@ -624,7 +624,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -677,14 +677,6 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -705,7 +697,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -767,26 +759,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -878,424 +856,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="35">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1476,6 +1042,418 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1490,22 +1468,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:J60" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J60"/>
-  <sortState ref="A2:J60">
-    <sortCondition ref="A1:A60"/>
-  </sortState>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:J62" headerRowDxfId="34" dataDxfId="33">
+  <autoFilter ref="A1:J62"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="S.no" dataDxfId="9"/>
-    <tableColumn id="2" name="University " dataDxfId="8"/>
-    <tableColumn id="3" name="Department" dataDxfId="7"/>
-    <tableColumn id="4" name="Project Title" dataDxfId="6"/>
-    <tableColumn id="11" name="Application Name" dataDxfId="5"/>
-    <tableColumn id="5" name="Team Leader Name" dataDxfId="4"/>
-    <tableColumn id="6" name="Team Leader Roll No" dataDxfId="3"/>
-    <tableColumn id="7" name="Batch" dataDxfId="2"/>
-    <tableColumn id="8" name="Status" dataDxfId="1"/>
-    <tableColumn id="9" name="Remarks" dataDxfId="0"/>
+    <tableColumn id="1" name="S.no" dataDxfId="32"/>
+    <tableColumn id="2" name="University " dataDxfId="31"/>
+    <tableColumn id="3" name="Department" dataDxfId="23"/>
+    <tableColumn id="4" name="Project Title" dataDxfId="30"/>
+    <tableColumn id="11" name="Application Name" dataDxfId="29"/>
+    <tableColumn id="5" name="Team Leader Name" dataDxfId="28"/>
+    <tableColumn id="6" name="Team Leader Roll No" dataDxfId="24"/>
+    <tableColumn id="7" name="Batch" dataDxfId="27"/>
+    <tableColumn id="8" name="Status" dataDxfId="26"/>
+    <tableColumn id="9" name="Remarks" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1777,11 +1752,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L145"/>
+  <dimension ref="A1:L149"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H60" sqref="H60"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1802,7 +1777,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -1814,7 +1789,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>3</v>
@@ -1823,7 +1798,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>5</v>
@@ -1843,7 +1818,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="E2" s="17"/>
       <c r="F2" s="15" t="s">
@@ -1853,7 +1828,7 @@
         <v>10</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I2" s="15" t="s">
         <v>13</v>
@@ -1871,17 +1846,17 @@
         <v>8</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E3" s="17"/>
       <c r="F3" s="15" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G3" s="18" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I3" s="15" t="s">
         <v>13</v>
@@ -1899,7 +1874,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="E4" s="17"/>
       <c r="F4" s="15" t="s">
@@ -1909,7 +1884,7 @@
         <v>15</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I4" s="15" t="s">
         <v>13</v>
@@ -1927,7 +1902,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="15" t="s">
@@ -1937,7 +1912,7 @@
         <v>17</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I5" s="15" t="s">
         <v>13</v>
@@ -1955,17 +1930,17 @@
         <v>8</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E6" s="17"/>
       <c r="F6" s="15" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G6" s="18" t="s">
         <v>19</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I6" s="15" t="s">
         <v>13</v>
@@ -1983,17 +1958,17 @@
         <v>8</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E7" s="17"/>
       <c r="F7" s="15" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G7" s="18" t="s">
         <v>20</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I7" s="15" t="s">
         <v>13</v>
@@ -2011,17 +1986,17 @@
         <v>8</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="15" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G8" s="18" t="s">
         <v>21</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I8" s="15" t="s">
         <v>13</v>
@@ -2039,7 +2014,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E9" s="17"/>
       <c r="F9" s="15" t="s">
@@ -2049,7 +2024,7 @@
         <v>23</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I9" s="15" t="s">
         <v>13</v>
@@ -2067,17 +2042,17 @@
         <v>8</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E10" s="17"/>
       <c r="F10" s="15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G10" s="18" t="s">
         <v>25</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I10" s="15" t="s">
         <v>13</v>
@@ -2095,17 +2070,17 @@
         <v>8</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E11" s="17"/>
       <c r="F11" s="15" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G11" s="18" t="s">
         <v>26</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I11" s="15" t="s">
         <v>13</v>
@@ -2123,7 +2098,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="15" t="s">
@@ -2133,7 +2108,7 @@
         <v>29</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I12" s="15" t="s">
         <v>13</v>
@@ -2151,7 +2126,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="20" t="str">
@@ -2162,7 +2137,7 @@
         <v>30</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I13" s="15" t="s">
         <v>13</v>
@@ -2180,17 +2155,17 @@
         <v>8</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="19" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="G14" s="18" t="s">
         <v>31</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I14" s="15" t="s">
         <v>13</v>
@@ -2208,17 +2183,17 @@
         <v>8</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E15" s="17"/>
       <c r="F15" s="15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G15" s="18" t="s">
         <v>32</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I15" s="15" t="s">
         <v>13</v>
@@ -2236,17 +2211,17 @@
         <v>8</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="E16" s="17"/>
       <c r="F16" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G16" s="18" t="s">
         <v>33</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I16" s="15" t="s">
         <v>13</v>
@@ -2264,24 +2239,24 @@
         <v>8</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E17" s="17"/>
       <c r="F17" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G17" s="18" t="s">
         <v>34</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I17" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J17" s="20"/>
     </row>
-    <row r="18" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14">
         <v>18</v>
       </c>
@@ -2292,17 +2267,17 @@
         <v>8</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G18" s="18" t="s">
         <v>36</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I18" s="15" t="s">
         <v>13</v>
@@ -2320,17 +2295,17 @@
         <v>8</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="15" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G19" s="18" t="s">
         <v>42</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I19" s="15" t="s">
         <v>13</v>
@@ -2348,17 +2323,17 @@
         <v>8</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="15" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G20" s="18" t="s">
         <v>43</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I20" s="15" t="s">
         <v>13</v>
@@ -2367,7 +2342,7 @@
     </row>
     <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>7</v>
@@ -2376,26 +2351,28 @@
         <v>8</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>178</v>
+        <v>150</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="15" t="s">
         <v>93</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>125</v>
+        <v>44</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J21" s="22"/>
-    </row>
-    <row r="22" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="J21" s="21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>7</v>
@@ -2404,28 +2381,26 @@
         <v>8</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>180</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="E22" s="17"/>
       <c r="F22" s="15" t="s">
         <v>94</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>179</v>
+        <v>128</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I22" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="J22" s="20"/>
+      <c r="J22" s="22"/>
     </row>
     <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>7</v>
@@ -2434,17 +2409,19 @@
         <v>8</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="E23" s="17"/>
+        <v>151</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>187</v>
+      </c>
       <c r="F23" s="15" t="s">
         <v>95</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>50</v>
+        <v>186</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I23" s="15" t="s">
         <v>13</v>
@@ -2453,7 +2430,7 @@
     </row>
     <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="15" t="s">
         <v>7</v>
@@ -2462,7 +2439,7 @@
         <v>8</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="15" t="s">
@@ -2472,7 +2449,7 @@
         <v>51</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I24" s="15" t="s">
         <v>13</v>
@@ -2481,7 +2458,7 @@
     </row>
     <row r="25" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="14">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" s="15" t="s">
         <v>7</v>
@@ -2490,17 +2467,17 @@
         <v>8</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="15" t="s">
         <v>97</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I25" s="15" t="s">
         <v>13</v>
@@ -2509,7 +2486,7 @@
     </row>
     <row r="26" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="14">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>7</v>
@@ -2518,7 +2495,7 @@
         <v>8</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="15" t="s">
@@ -2528,7 +2505,7 @@
         <v>55</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I26" s="15" t="s">
         <v>13</v>
@@ -2537,7 +2514,7 @@
     </row>
     <row r="27" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="14">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>7</v>
@@ -2546,17 +2523,17 @@
         <v>8</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="15" t="s">
         <v>99</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I27" s="15" t="s">
         <v>13</v>
@@ -2565,7 +2542,7 @@
     </row>
     <row r="28" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="14">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>7</v>
@@ -2574,7 +2551,7 @@
         <v>8</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="15" t="s">
@@ -2584,7 +2561,7 @@
         <v>73</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I28" s="15" t="s">
         <v>13</v>
@@ -2593,7 +2570,7 @@
     </row>
     <row r="29" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="14">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>7</v>
@@ -2602,14 +2579,14 @@
         <v>8</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="15" t="s">
         <v>101</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="H29" s="15" t="s">
         <v>69</v>
@@ -2621,7 +2598,7 @@
     </row>
     <row r="30" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="14">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" s="15" t="s">
         <v>7</v>
@@ -2630,17 +2607,17 @@
         <v>8</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="15" t="s">
         <v>102</v>
       </c>
       <c r="G30" s="18" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I30" s="15" t="s">
         <v>13</v>
@@ -2649,7 +2626,7 @@
     </row>
     <row r="31" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="14">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31" s="15" t="s">
         <v>7</v>
@@ -2658,26 +2635,26 @@
         <v>8</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>127</v>
+        <v>159</v>
       </c>
       <c r="E31" s="17"/>
       <c r="F31" s="15" t="s">
         <v>103</v>
       </c>
       <c r="G31" s="18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I31" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="J31" s="22"/>
+      <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="14">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32" s="15" t="s">
         <v>7</v>
@@ -2686,26 +2663,26 @@
         <v>8</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
       <c r="E32" s="17"/>
       <c r="F32" s="15" t="s">
         <v>104</v>
       </c>
       <c r="G32" s="18" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I32" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="J32" s="20"/>
+      <c r="J32" s="22"/>
     </row>
     <row r="33" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="14">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B33" s="15" t="s">
         <v>7</v>
@@ -2714,17 +2691,17 @@
         <v>8</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E33" s="17"/>
       <c r="F33" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G33" s="18" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I33" s="15" t="s">
         <v>13</v>
@@ -2733,7 +2710,7 @@
     </row>
     <row r="34" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="14">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B34" s="15" t="s">
         <v>7</v>
@@ -2742,26 +2719,28 @@
         <v>8</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E34" s="17"/>
       <c r="F34" s="15" t="s">
-        <v>40</v>
+        <v>106</v>
       </c>
       <c r="G34" s="18" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I34" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J34" s="20"/>
+        <v>11</v>
+      </c>
+      <c r="J34" s="21" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="35" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="14">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B35" s="15" t="s">
         <v>7</v>
@@ -2770,28 +2749,26 @@
         <v>8</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E35" s="17"/>
       <c r="F35" s="15" t="s">
         <v>107</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I35" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J35" s="21" t="s">
-        <v>45</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="J35" s="20"/>
     </row>
     <row r="36" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="14">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B36" s="15" t="s">
         <v>7</v>
@@ -2800,17 +2777,17 @@
         <v>8</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="E36" s="17"/>
       <c r="F36" s="15" t="s">
-        <v>108</v>
+        <v>40</v>
       </c>
       <c r="G36" s="18" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I36" s="15" t="s">
         <v>13</v>
@@ -2819,7 +2796,7 @@
     </row>
     <row r="37" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="14">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B37" s="15" t="s">
         <v>7</v>
@@ -2828,26 +2805,28 @@
         <v>8</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E37" s="17"/>
       <c r="F37" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G37" s="18" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H37" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J37" s="20"/>
+        <v>11</v>
+      </c>
+      <c r="J37" s="21" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="38" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="14">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B38" s="15" t="s">
         <v>7</v>
@@ -2856,26 +2835,28 @@
         <v>8</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E38" s="17"/>
       <c r="F38" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G38" s="18" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I38" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J38" s="20"/>
+        <v>11</v>
+      </c>
+      <c r="J38" s="21" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="14">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B39" s="15" t="s">
         <v>7</v>
@@ -2884,17 +2865,17 @@
         <v>8</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="E39" s="17"/>
       <c r="F39" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G39" s="18" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I39" s="15" t="s">
         <v>13</v>
@@ -2903,7 +2884,7 @@
     </row>
     <row r="40" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="14">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B40" s="15" t="s">
         <v>7</v>
@@ -2912,26 +2893,28 @@
         <v>8</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E40" s="17"/>
       <c r="F40" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G40" s="18" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I40" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J40" s="20"/>
+        <v>11</v>
+      </c>
+      <c r="J40" s="21" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="14">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B41" s="15" t="s">
         <v>7</v>
@@ -2940,28 +2923,26 @@
         <v>8</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E41" s="17"/>
       <c r="F41" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G41" s="18" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I41" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J41" s="21" t="s">
-        <v>66</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="J41" s="20"/>
     </row>
     <row r="42" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="14">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B42" s="15" t="s">
         <v>7</v>
@@ -2970,17 +2951,17 @@
         <v>8</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E42" s="17"/>
       <c r="F42" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G42" s="18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H42" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I42" s="15" t="s">
         <v>13</v>
@@ -2989,7 +2970,7 @@
     </row>
     <row r="43" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="14">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B43" s="15" t="s">
         <v>7</v>
@@ -2998,17 +2979,17 @@
         <v>8</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="E43" s="17"/>
       <c r="F43" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G43" s="18" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="H43" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I43" s="15" t="s">
         <v>13</v>
@@ -3017,7 +2998,7 @@
     </row>
     <row r="44" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="14">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B44" s="15" t="s">
         <v>7</v>
@@ -3026,17 +3007,17 @@
         <v>8</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E44" s="17"/>
       <c r="F44" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G44" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H44" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I44" s="15" t="s">
         <v>13</v>
@@ -3045,7 +3026,7 @@
     </row>
     <row r="45" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="14">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B45" s="15" t="s">
         <v>7</v>
@@ -3054,26 +3035,28 @@
         <v>8</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="E45" s="17"/>
       <c r="F45" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G45" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H45" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I45" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J45" s="20"/>
-    </row>
-    <row r="46" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="J45" s="21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="14">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B46" s="15" t="s">
         <v>7</v>
@@ -3082,17 +3065,17 @@
         <v>8</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="E46" s="17"/>
       <c r="F46" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G46" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H46" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I46" s="15" t="s">
         <v>13</v>
@@ -3101,7 +3084,7 @@
     </row>
     <row r="47" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="14">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B47" s="15" t="s">
         <v>7</v>
@@ -3110,17 +3093,17 @@
         <v>8</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="E47" s="17"/>
       <c r="F47" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G47" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H47" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I47" s="15" t="s">
         <v>13</v>
@@ -3129,7 +3112,7 @@
     </row>
     <row r="48" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="14">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B48" s="15" t="s">
         <v>7</v>
@@ -3138,17 +3121,17 @@
         <v>8</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="E48" s="17"/>
       <c r="F48" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G48" s="18" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="H48" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I48" s="15" t="s">
         <v>13</v>
@@ -3157,7 +3140,7 @@
     </row>
     <row r="49" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="14">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B49" s="15" t="s">
         <v>7</v>
@@ -3166,26 +3149,26 @@
         <v>8</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E49" s="17"/>
       <c r="F49" s="15" t="s">
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="G49" s="18" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I49" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J49" s="20"/>
     </row>
-    <row r="50" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A50" s="14">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B50" s="15" t="s">
         <v>7</v>
@@ -3194,17 +3177,17 @@
         <v>8</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E50" s="17"/>
       <c r="F50" s="15" t="s">
         <v>121</v>
       </c>
       <c r="G50" s="18" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H50" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I50" s="15" t="s">
         <v>13</v>
@@ -3213,7 +3196,7 @@
     </row>
     <row r="51" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="14">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B51" s="15" t="s">
         <v>7</v>
@@ -3222,17 +3205,17 @@
         <v>8</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E51" s="17"/>
       <c r="F51" s="15" t="s">
         <v>122</v>
       </c>
       <c r="G51" s="18" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="H51" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I51" s="15" t="s">
         <v>13</v>
@@ -3241,7 +3224,7 @@
     </row>
     <row r="52" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="14">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B52" s="15" t="s">
         <v>7</v>
@@ -3249,177 +3232,169 @@
       <c r="C52" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D52" s="20" t="s">
-        <v>175</v>
+      <c r="D52" s="16" t="s">
+        <v>178</v>
       </c>
       <c r="E52" s="17"/>
       <c r="F52" s="15" t="s">
         <v>123</v>
       </c>
       <c r="G52" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="H52" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="I52" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J52" s="20"/>
+    </row>
+    <row r="53" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="14">
+        <v>55</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="E53" s="17"/>
+      <c r="F53" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G53" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="H53" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="I53" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J53" s="20"/>
+    </row>
+    <row r="54" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="14">
+        <v>56</v>
+      </c>
+      <c r="B54" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="E54" s="17"/>
+      <c r="F54" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="G54" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="H52" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="I52" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J52" s="21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="14">
-        <v>59</v>
-      </c>
-      <c r="B53" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D53" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="E53" s="19"/>
-      <c r="F53" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="G53" s="18" t="s">
+      <c r="H54" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="I54" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J54" s="20"/>
+    </row>
+    <row r="55" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="14">
+        <v>57</v>
+      </c>
+      <c r="B55" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="E55" s="17"/>
+      <c r="F55" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="G55" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="H55" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="I55" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J55" s="20"/>
+    </row>
+    <row r="56" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="14">
+        <v>58</v>
+      </c>
+      <c r="B56" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="E56" s="17"/>
+      <c r="F56" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="G56" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="H53" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="I53" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J53" s="20"/>
-    </row>
-    <row r="54" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="24">
-        <v>60</v>
-      </c>
-      <c r="B54" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C54" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D54" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="E54" s="26"/>
-      <c r="F54" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="G54" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="H54" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="I54" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J54" s="20"/>
-    </row>
-    <row r="55" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="24">
-        <v>61</v>
-      </c>
-      <c r="B55" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D55" s="25" t="s">
-        <v>186</v>
-      </c>
-      <c r="E55" s="26"/>
-      <c r="F55" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="G55" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="H55" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="I55" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J55" s="20"/>
-      <c r="K55" s="5"/>
-      <c r="L55" s="5"/>
-    </row>
-    <row r="56" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="24">
-        <v>62</v>
-      </c>
-      <c r="B56" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D56" s="31" t="s">
-        <v>182</v>
-      </c>
-      <c r="E56" s="26"/>
-      <c r="F56" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="G56" s="28" t="s">
-        <v>46</v>
-      </c>
       <c r="H56" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I56" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="J56" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="K56" s="5"/>
-      <c r="L56" s="5"/>
+      <c r="J56" s="21" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="57" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="24">
-        <v>63</v>
-      </c>
-      <c r="B57" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C57" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D57" s="31" t="s">
-        <v>187</v>
-      </c>
-      <c r="E57" s="26"/>
-      <c r="F57" s="25" t="s">
-        <v>189</v>
-      </c>
-      <c r="G57" s="28" t="s">
+      <c r="A57" s="14">
+        <v>59</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" s="20" t="s">
         <v>183</v>
       </c>
+      <c r="E57" s="19"/>
+      <c r="F57" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="G57" s="18" t="s">
+        <v>66</v>
+      </c>
       <c r="H57" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I57" s="15" t="s">
         <v>13</v>
       </c>
       <c r="J57" s="20"/>
-      <c r="K57" s="5"/>
-      <c r="L57" s="5"/>
     </row>
     <row r="58" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="24">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B58" s="25" t="s">
         <v>7</v>
@@ -3427,31 +3402,27 @@
       <c r="C58" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D58" s="31" t="s">
-        <v>184</v>
+      <c r="D58" s="25" t="s">
+        <v>192</v>
       </c>
       <c r="E58" s="26"/>
       <c r="F58" s="25" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="G58" s="28" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="H58" s="15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I58" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J58" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="K58" s="5"/>
-      <c r="L58" s="5"/>
-    </row>
-    <row r="59" spans="1:12" s="36" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="J58" s="20"/>
+    </row>
+    <row r="59" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="24">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B59" s="25" t="s">
         <v>7</v>
@@ -3459,73 +3430,117 @@
       <c r="C59" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D59" s="33" t="s">
-        <v>194</v>
+      <c r="D59" s="25" t="s">
+        <v>193</v>
       </c>
       <c r="E59" s="26"/>
       <c r="F59" s="25" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="G59" s="28" t="s">
-        <v>190</v>
-      </c>
-      <c r="H59" s="34" t="s">
-        <v>191</v>
-      </c>
-      <c r="I59" s="25" t="s">
-        <v>196</v>
-      </c>
-      <c r="J59" s="31"/>
-      <c r="K59" s="35"/>
-      <c r="L59" s="35"/>
-    </row>
-    <row r="60" spans="1:12" s="36" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="H59" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="I59" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J59" s="20"/>
+      <c r="K59" s="5"/>
+      <c r="L59" s="5"/>
+    </row>
+    <row r="60" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="24">
-        <v>66</v>
-      </c>
-      <c r="B60" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="C60" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="D60" s="39" t="s">
-        <v>195</v>
+        <v>62</v>
+      </c>
+      <c r="B60" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" s="31" t="s">
+        <v>189</v>
       </c>
       <c r="E60" s="26"/>
       <c r="F60" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="G60" s="38" t="s">
+        <v>195</v>
+      </c>
+      <c r="G60" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H60" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="I60" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J60" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="K60" s="5"/>
+      <c r="L60" s="5"/>
+    </row>
+    <row r="61" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="24">
+        <v>63</v>
+      </c>
+      <c r="B61" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" s="31" t="s">
+        <v>194</v>
+      </c>
+      <c r="E61" s="26"/>
+      <c r="F61" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="G61" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="H61" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="I61" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J61" s="20"/>
+      <c r="K61" s="5"/>
+      <c r="L61" s="5"/>
+    </row>
+    <row r="62" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="24">
         <v>64</v>
       </c>
-      <c r="H60" s="40" t="s">
-        <v>192</v>
-      </c>
-      <c r="I60" s="25" t="s">
-        <v>196</v>
-      </c>
-      <c r="J60" s="41"/>
-      <c r="K60" s="35"/>
-      <c r="L60" s="35"/>
-    </row>
-    <row r="61" spans="1:12" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="42"/>
-      <c r="C61" s="43"/>
-      <c r="D61" s="44"/>
-      <c r="E61" s="45"/>
-      <c r="G61" s="46"/>
-      <c r="H61" s="35"/>
-      <c r="I61" s="35"/>
-      <c r="J61" s="47"/>
-      <c r="K61" s="35"/>
-      <c r="L61" s="35"/>
-    </row>
-    <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G62" s="29"/>
-      <c r="H62" s="5"/>
-      <c r="I62" s="5"/>
-      <c r="J62" s="6"/>
+      <c r="B62" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" s="31" t="s">
+        <v>191</v>
+      </c>
+      <c r="E62" s="26"/>
+      <c r="F62" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="G62" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="H62" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="I62" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J62" s="23" t="s">
+        <v>67</v>
+      </c>
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
     </row>
@@ -4193,72 +4208,97 @@
       <c r="K145" s="5"/>
       <c r="L145" s="5"/>
     </row>
+    <row r="146" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G146" s="29"/>
+      <c r="H146" s="5"/>
+      <c r="I146" s="5"/>
+      <c r="J146" s="6"/>
+      <c r="K146" s="5"/>
+      <c r="L146" s="5"/>
+    </row>
+    <row r="147" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G147" s="29"/>
+      <c r="H147" s="5"/>
+      <c r="I147" s="5"/>
+      <c r="J147" s="6"/>
+      <c r="K147" s="5"/>
+      <c r="L147" s="5"/>
+    </row>
+    <row r="148" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G148" s="29"/>
+      <c r="H148" s="5"/>
+      <c r="I148" s="5"/>
+      <c r="J148" s="6"/>
+      <c r="K148" s="5"/>
+      <c r="L148" s="5"/>
+    </row>
+    <row r="149" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G149" s="29"/>
+      <c r="H149" s="5"/>
+      <c r="I149" s="5"/>
+      <c r="J149" s="6"/>
+      <c r="K149" s="5"/>
+      <c r="L149" s="5"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="I1 I54:I1048576">
-    <cfRule type="containsText" dxfId="30" priority="23" operator="containsText" text="Pending">
+  <conditionalFormatting sqref="I1 I58:I1048576">
+    <cfRule type="containsText" dxfId="17" priority="22" operator="containsText" text="Pending">
       <formula>NOT(ISERROR(SEARCH("Pending",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="24" operator="containsText" text="Accepted">
+    <cfRule type="containsText" dxfId="16" priority="23" operator="containsText" text="Accepted">
       <formula>NOT(ISERROR(SEARCH("Accepted",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="25" operator="containsText" text="Rejected">
+    <cfRule type="containsText" dxfId="15" priority="24" operator="containsText" text="Rejected">
       <formula>NOT(ISERROR(SEARCH("Rejected",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G146:G1048576 G1">
-    <cfRule type="duplicateValues" dxfId="27" priority="18"/>
-    <cfRule type="duplicateValues" dxfId="26" priority="22"/>
-    <cfRule type="duplicateValues" dxfId="25" priority="26"/>
+  <conditionalFormatting sqref="G1 G150:G1048576">
+    <cfRule type="duplicateValues" dxfId="14" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="25"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F61:F1048576 F1">
-    <cfRule type="duplicateValues" dxfId="24" priority="17"/>
+  <conditionalFormatting sqref="F63:F1048576 F1">
+    <cfRule type="duplicateValues" dxfId="11" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="duplicateValues" dxfId="23" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="containsText" dxfId="22" priority="15" operator="containsText" text="Rejected">
+    <cfRule type="containsText" dxfId="9" priority="14" operator="containsText" text="Rejected">
       <formula>NOT(ISERROR(SEARCH("Rejected",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="16" operator="containsText" text="Accepted">
+    <cfRule type="containsText" dxfId="8" priority="15" operator="containsText" text="Accepted">
       <formula>NOT(ISERROR(SEARCH("Accepted",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G146:G1048576 G1:G53">
-    <cfRule type="duplicateValues" dxfId="20" priority="9"/>
+  <conditionalFormatting sqref="G150:G1048576 G1:G57">
+    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G63">
-    <cfRule type="duplicateValues" dxfId="19" priority="4"/>
+  <conditionalFormatting sqref="G67">
+    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G113">
-    <cfRule type="duplicateValues" dxfId="18" priority="5"/>
+  <conditionalFormatting sqref="G117">
+    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G119 G140:G141 G132 G61">
-    <cfRule type="duplicateValues" dxfId="17" priority="6"/>
+  <conditionalFormatting sqref="G123 G144:G145 G136 G65">
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G144 G142 G120 G137:G139 G133:G135 G122:G131 G114:G118 G65:G112 G62">
-    <cfRule type="duplicateValues" dxfId="16" priority="8"/>
+  <conditionalFormatting sqref="G148 G146 G124 G141:G143 G137:G139 G126:G135 G118:G122 G69:G116 G63:G64 G66">
+    <cfRule type="duplicateValues" dxfId="3" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G145 G143 G121 G136 G64">
-    <cfRule type="duplicateValues" dxfId="15" priority="7"/>
+  <conditionalFormatting sqref="G149 G147 G125 G140 G68">
+    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G61:G1048576 G1:G53">
-    <cfRule type="duplicateValues" dxfId="14" priority="3"/>
+  <conditionalFormatting sqref="G1:G57 G63:G1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D61:D1048576 D1">
-    <cfRule type="duplicateValues" dxfId="13" priority="2"/>
+  <conditionalFormatting sqref="D63:D1048576 D1">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
-  </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="H59" r:id="rId1"/>
-    <hyperlink ref="H60" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
form handling updated with all CURD operations and form validations
</commit_message>
<xml_diff>
--- a/project/MRU Java FSD Project Final.xlsx
+++ b/project/MRU Java FSD Project Final.xlsx
@@ -861,7 +861,17 @@
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="31">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1044,112 +1054,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1248,6 +1152,34 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1355,6 +1287,34 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1468,19 +1428,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:J62" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:J62" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="A1:J62"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="S.no" dataDxfId="32"/>
-    <tableColumn id="2" name="University " dataDxfId="31"/>
-    <tableColumn id="3" name="Department" dataDxfId="23"/>
-    <tableColumn id="4" name="Project Title" dataDxfId="30"/>
-    <tableColumn id="11" name="Application Name" dataDxfId="29"/>
-    <tableColumn id="5" name="Team Leader Name" dataDxfId="28"/>
-    <tableColumn id="6" name="Team Leader Roll No" dataDxfId="24"/>
-    <tableColumn id="7" name="Batch" dataDxfId="27"/>
-    <tableColumn id="8" name="Status" dataDxfId="26"/>
-    <tableColumn id="9" name="Remarks" dataDxfId="25"/>
+    <tableColumn id="1" name="S.no" dataDxfId="28"/>
+    <tableColumn id="2" name="University " dataDxfId="27"/>
+    <tableColumn id="3" name="Department" dataDxfId="26"/>
+    <tableColumn id="4" name="Project Title" dataDxfId="25"/>
+    <tableColumn id="11" name="Application Name" dataDxfId="24"/>
+    <tableColumn id="5" name="Team Leader Name" dataDxfId="23"/>
+    <tableColumn id="6" name="Team Leader Roll No" dataDxfId="22"/>
+    <tableColumn id="7" name="Batch" dataDxfId="21"/>
+    <tableColumn id="8" name="Status" dataDxfId="20"/>
+    <tableColumn id="9" name="Remarks" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1755,8 +1715,8 @@
   <dimension ref="A1:L149"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F65" sqref="F65"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4242,57 +4202,60 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1 I58:I1048576">
-    <cfRule type="containsText" dxfId="17" priority="22" operator="containsText" text="Pending">
+    <cfRule type="containsText" dxfId="18" priority="23" operator="containsText" text="Pending">
       <formula>NOT(ISERROR(SEARCH("Pending",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="23" operator="containsText" text="Accepted">
+    <cfRule type="containsText" dxfId="17" priority="24" operator="containsText" text="Accepted">
       <formula>NOT(ISERROR(SEARCH("Accepted",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="24" operator="containsText" text="Rejected">
+    <cfRule type="containsText" dxfId="16" priority="25" operator="containsText" text="Rejected">
       <formula>NOT(ISERROR(SEARCH("Rejected",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1 G150:G1048576">
-    <cfRule type="duplicateValues" dxfId="14" priority="17"/>
-    <cfRule type="duplicateValues" dxfId="13" priority="21"/>
-    <cfRule type="duplicateValues" dxfId="12" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F63:F1048576 F1">
-    <cfRule type="duplicateValues" dxfId="11" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="duplicateValues" dxfId="10" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="containsText" dxfId="9" priority="14" operator="containsText" text="Rejected">
+    <cfRule type="containsText" dxfId="10" priority="15" operator="containsText" text="Rejected">
       <formula>NOT(ISERROR(SEARCH("Rejected",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="15" operator="containsText" text="Accepted">
+    <cfRule type="containsText" dxfId="9" priority="16" operator="containsText" text="Accepted">
       <formula>NOT(ISERROR(SEARCH("Accepted",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G150:G1048576 G1:G57">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G67">
-    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G117">
-    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G123 G144:G145 G136 G65">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G148 G146 G124 G141:G143 G137:G139 G126:G135 G118:G122 G69:G116 G63:G64 G66">
+    <cfRule type="duplicateValues" dxfId="4" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G149 G147 G125 G140 G68">
     <cfRule type="duplicateValues" dxfId="3" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G149 G147 G125 G140 G68">
-    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
+  <conditionalFormatting sqref="G1:G57 G63:G1048576">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G57 G63:G1048576">
+  <conditionalFormatting sqref="D63:D1048576 D1">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D63:D1048576 D1">
+  <conditionalFormatting sqref="G1:G1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
react basics: form handling final with curd
</commit_message>
<xml_diff>
--- a/project/MRU Java FSD Project Final.xlsx
+++ b/project/MRU Java FSD Project Final.xlsx
@@ -593,10 +593,10 @@
     <t>Crowdsourced Disaster Relief App</t>
   </si>
   <si>
-    <t>Smart Waste Management</t>
-  </si>
-  <si>
     <t>2211CS030110</t>
+  </si>
+  <si>
+    <t>Integrated Waste Management &amp; Awareness Platform</t>
   </si>
 </sst>
 </file>
@@ -606,7 +606,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -675,6 +675,13 @@
     </font>
     <font>
       <sz val="13.5"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -781,7 +788,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -896,6 +903,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1768,7 +1778,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G60" sqref="G60"/>
+      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3322,8 +3332,8 @@
       <c r="C55" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D55" s="31" t="s">
-        <v>189</v>
+      <c r="D55" s="41" t="s">
+        <v>190</v>
       </c>
       <c r="E55" s="26"/>
       <c r="F55" s="25" t="s">
@@ -3450,7 +3460,7 @@
         <v>121</v>
       </c>
       <c r="G59" s="28" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H59" s="15" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
React Router: examples added, Project Proposal: updated
</commit_message>
<xml_diff>
--- a/project/MRU Java FSD Project Final.xlsx
+++ b/project/MRU Java FSD Project Final.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="188">
   <si>
     <t xml:space="preserve">University </t>
   </si>
@@ -59,9 +59,6 @@
     <t>2211CS030073</t>
   </si>
   <si>
-    <t>Rejected</t>
-  </si>
-  <si>
     <t>2211CS030011</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>2211CS030051</t>
   </si>
   <si>
-    <t>Over Exhaused and Lack of Innovative ideas.</t>
-  </si>
-  <si>
     <t>2211CS030170</t>
   </si>
   <si>
@@ -218,9 +212,6 @@
     <t>2211CS030149</t>
   </si>
   <si>
-    <t>Title Taken</t>
-  </si>
-  <si>
     <t>Batch</t>
   </si>
   <si>
@@ -497,9 +488,6 @@
     <t>INVENTORY MANAGEMENT</t>
   </si>
   <si>
-    <t xml:space="preserve">TASK MANAGER </t>
-  </si>
-  <si>
     <t>REAL-TIME MULTIPLAYER CHESS GAME</t>
   </si>
   <si>
@@ -515,9 +503,6 @@
     <t>FASHION SUSTAINABILITY HUB</t>
   </si>
   <si>
-    <t>ECHOBEAT</t>
-  </si>
-  <si>
     <t>SMART KNOWLEDGE HUB</t>
   </si>
   <si>
@@ -566,9 +551,6 @@
     <t>2211CS030128</t>
   </si>
   <si>
-    <t>NUTRITION COUNT</t>
-  </si>
-  <si>
     <t>BLOOD AND ORGAN DONATION PLATFORM</t>
   </si>
   <si>
@@ -597,6 +579,15 @@
   </si>
   <si>
     <t>Integrated Waste Management &amp; Awareness Platform</t>
+  </si>
+  <si>
+    <t>Peer-to-Peer Lending Platform</t>
+  </si>
+  <si>
+    <t>REAL TIME SPORTS SCORE</t>
+  </si>
+  <si>
+    <t>HOME COOK SERVICE MANAGEMENT</t>
   </si>
 </sst>
 </file>
@@ -606,7 +597,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -683,6 +674,20 @@
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -844,13 +849,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -905,6 +904,12 @@
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1776,20 +1781,20 @@
   </sheetPr>
   <dimension ref="A1:L144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" style="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" style="30" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="63.109375" style="13" customWidth="1"/>
     <col min="5" max="5" width="23.77734375" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.88671875" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.88671875" style="28" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="66.6640625" style="2" customWidth="1"/>
@@ -1799,7 +1804,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -1811,16 +1816,16 @@
         <v>2</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="25" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>5</v>
@@ -1840,7 +1845,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E2" s="17"/>
       <c r="F2" s="15" t="s">
@@ -1850,10 +1855,10 @@
         <v>10</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J2" s="20"/>
     </row>
@@ -1868,20 +1873,20 @@
         <v>8</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E3" s="17"/>
       <c r="F3" s="15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J3" s="20"/>
     </row>
@@ -1896,20 +1901,20 @@
         <v>8</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E4" s="17"/>
       <c r="F4" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="18" t="s">
-        <v>15</v>
-      </c>
       <c r="H4" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J4" s="20"/>
     </row>
@@ -1924,20 +1929,20 @@
         <v>8</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="18" t="s">
-        <v>17</v>
-      </c>
       <c r="H5" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J5" s="20"/>
     </row>
@@ -1952,20 +1957,20 @@
         <v>8</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E6" s="17"/>
       <c r="F6" s="15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J6" s="20"/>
     </row>
@@ -1980,20 +1985,20 @@
         <v>8</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E7" s="17"/>
       <c r="F7" s="15" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J7" s="20"/>
     </row>
@@ -2008,20 +2013,20 @@
         <v>8</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J8" s="20"/>
     </row>
@@ -2036,20 +2041,20 @@
         <v>8</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E9" s="17"/>
       <c r="F9" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="18" t="s">
-        <v>23</v>
-      </c>
       <c r="H9" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J9" s="20"/>
     </row>
@@ -2064,20 +2069,20 @@
         <v>8</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E10" s="17"/>
       <c r="F10" s="15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J10" s="20"/>
     </row>
@@ -2092,20 +2097,20 @@
         <v>8</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E11" s="17"/>
       <c r="F11" s="15" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J11" s="20"/>
     </row>
@@ -2120,20 +2125,20 @@
         <v>8</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="18" t="s">
-        <v>29</v>
-      </c>
       <c r="H12" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J12" s="20"/>
     </row>
@@ -2148,7 +2153,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="20" t="str">
@@ -2156,13 +2161,13 @@
         <v>G.SAI KAVYA</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J13" s="20"/>
     </row>
@@ -2177,20 +2182,20 @@
         <v>8</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="19" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J14" s="20"/>
     </row>
@@ -2205,20 +2210,20 @@
         <v>8</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E15" s="17"/>
       <c r="F15" s="15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J15" s="20"/>
     </row>
@@ -2233,20 +2238,20 @@
         <v>8</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E16" s="17"/>
       <c r="F16" s="15" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J16" s="20"/>
     </row>
@@ -2261,20 +2266,20 @@
         <v>8</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E17" s="17"/>
       <c r="F17" s="15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J17" s="20"/>
     </row>
@@ -2289,20 +2294,20 @@
         <v>8</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="15" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J18" s="20"/>
     </row>
@@ -2317,20 +2322,20 @@
         <v>8</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="15" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J19" s="20"/>
     </row>
@@ -2345,20 +2350,20 @@
         <v>8</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="15" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J20" s="20"/>
     </row>
@@ -2373,22 +2378,22 @@
         <v>8</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="15" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J21" s="22"/>
+        <v>12</v>
+      </c>
+      <c r="J21" s="21"/>
     </row>
     <row r="22" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14">
@@ -2401,22 +2406,22 @@
         <v>8</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J22" s="20"/>
     </row>
@@ -2431,20 +2436,20 @@
         <v>8</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J23" s="20"/>
     </row>
@@ -2459,20 +2464,20 @@
         <v>8</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J24" s="20"/>
     </row>
@@ -2487,20 +2492,20 @@
         <v>8</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="15" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I25" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J25" s="20"/>
     </row>
@@ -2515,20 +2520,20 @@
         <v>8</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I26" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J26" s="20"/>
     </row>
@@ -2543,20 +2548,20 @@
         <v>8</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I27" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J27" s="20"/>
     </row>
@@ -2571,20 +2576,20 @@
         <v>8</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J28" s="20"/>
     </row>
@@ -2599,20 +2604,20 @@
         <v>8</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="15" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H29" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I29" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J29" s="20"/>
     </row>
@@ -2627,20 +2632,20 @@
         <v>8</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G30" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I30" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J30" s="20"/>
     </row>
@@ -2655,22 +2660,22 @@
         <v>8</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E31" s="17"/>
       <c r="F31" s="15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G31" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I31" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J31" s="22"/>
+        <v>12</v>
+      </c>
+      <c r="J31" s="21"/>
     </row>
     <row r="32" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="14">
@@ -2683,20 +2688,20 @@
         <v>8</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E32" s="17"/>
       <c r="F32" s="15" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G32" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I32" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J32" s="20"/>
     </row>
@@ -2711,20 +2716,20 @@
         <v>8</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E33" s="17"/>
       <c r="F33" s="15" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G33" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I33" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J33" s="20"/>
     </row>
@@ -2739,20 +2744,20 @@
         <v>8</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E34" s="17"/>
       <c r="F34" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G34" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="G34" s="18" t="s">
-        <v>40</v>
-      </c>
       <c r="H34" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I34" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J34" s="20"/>
     </row>
@@ -2767,24 +2772,22 @@
         <v>8</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>157</v>
+        <v>187</v>
       </c>
       <c r="E35" s="17"/>
       <c r="F35" s="15" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I35" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J35" s="21" t="s">
-        <v>44</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="J35"/>
     </row>
     <row r="36" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="14">
@@ -2797,20 +2800,20 @@
         <v>8</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E36" s="17"/>
       <c r="F36" s="15" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G36" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I36" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J36" s="20"/>
     </row>
@@ -2825,20 +2828,20 @@
         <v>8</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E37" s="17"/>
       <c r="F37" s="15" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G37" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H37" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J37" s="20"/>
     </row>
@@ -2853,20 +2856,20 @@
         <v>8</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E38" s="17"/>
       <c r="F38" s="15" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G38" s="18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I38" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J38" s="20"/>
     </row>
@@ -2881,20 +2884,20 @@
         <v>8</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E39" s="17"/>
       <c r="F39" s="15" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G39" s="18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I39" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J39" s="20"/>
     </row>
@@ -2909,20 +2912,20 @@
         <v>8</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E40" s="17"/>
       <c r="F40" s="15" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G40" s="18" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I40" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J40" s="20"/>
     </row>
@@ -2936,25 +2939,23 @@
       <c r="C41" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D41" s="16" t="s">
-        <v>163</v>
+      <c r="D41" s="38" t="s">
+        <v>185</v>
       </c>
       <c r="E41" s="17"/>
       <c r="F41" s="15" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G41" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I41" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J41" s="21" t="s">
-        <v>64</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="J41"/>
     </row>
     <row r="42" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="14">
@@ -2967,20 +2968,20 @@
         <v>8</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E42" s="17"/>
       <c r="F42" s="15" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G42" s="18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H42" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I42" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J42" s="20"/>
     </row>
@@ -2995,20 +2996,20 @@
         <v>8</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E43" s="17"/>
       <c r="F43" s="15" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G43" s="18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H43" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I43" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J43" s="20"/>
     </row>
@@ -3023,20 +3024,20 @@
         <v>8</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E44" s="17"/>
       <c r="F44" s="15" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G44" s="18" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H44" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I44" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J44" s="20"/>
     </row>
@@ -3051,20 +3052,20 @@
         <v>8</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E45" s="17"/>
       <c r="F45" s="15" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G45" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H45" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I45" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J45" s="20"/>
     </row>
@@ -3079,20 +3080,20 @@
         <v>8</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E46" s="17"/>
       <c r="F46" s="15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G46" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H46" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I46" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J46" s="20"/>
     </row>
@@ -3107,20 +3108,20 @@
         <v>8</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E47" s="17"/>
       <c r="F47" s="15" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G47" s="18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H47" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I47" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J47" s="20"/>
     </row>
@@ -3135,20 +3136,20 @@
         <v>8</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E48" s="17"/>
       <c r="F48" s="15" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G48" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H48" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I48" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J48" s="20"/>
     </row>
@@ -3163,20 +3164,20 @@
         <v>8</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E49" s="17"/>
       <c r="F49" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G49" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I49" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J49" s="20"/>
     </row>
@@ -3191,20 +3192,20 @@
         <v>8</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E50" s="17"/>
       <c r="F50" s="15" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G50" s="18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H50" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I50" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J50" s="20"/>
     </row>
@@ -3219,20 +3220,20 @@
         <v>8</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E51" s="17"/>
       <c r="F51" s="15" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G51" s="18" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H51" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I51" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J51" s="20"/>
     </row>
@@ -3247,233 +3248,231 @@
         <v>8</v>
       </c>
       <c r="D52" s="20" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E52" s="19"/>
       <c r="F52" s="15" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G52" s="18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H52" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I52" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J52" s="20"/>
     </row>
     <row r="53" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="24">
+      <c r="A53" s="22">
         <v>60</v>
       </c>
-      <c r="B53" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D53" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="E53" s="26"/>
-      <c r="F53" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="G53" s="28" t="s">
-        <v>43</v>
+      <c r="B53" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="E53" s="24"/>
+      <c r="F53" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="G53" s="26" t="s">
+        <v>42</v>
       </c>
       <c r="H53" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I53" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J53" s="20"/>
     </row>
     <row r="54" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="24">
+      <c r="A54" s="22">
         <v>61</v>
       </c>
-      <c r="B54" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C54" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D54" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="E54" s="26"/>
-      <c r="F54" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="G54" s="28" t="s">
-        <v>48</v>
+      <c r="B54" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="E54" s="24"/>
+      <c r="F54" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="G54" s="26" t="s">
+        <v>46</v>
       </c>
       <c r="H54" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I54" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J54" s="20"/>
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
     </row>
     <row r="55" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="24">
+      <c r="A55" s="22">
         <v>62</v>
       </c>
-      <c r="B55" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D55" s="41" t="s">
-        <v>190</v>
-      </c>
-      <c r="E55" s="26"/>
-      <c r="F55" s="25" t="s">
+      <c r="B55" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" s="39" t="s">
         <v>184</v>
       </c>
-      <c r="G55" s="28" t="s">
-        <v>45</v>
+      <c r="E55" s="24"/>
+      <c r="F55" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="G55" s="26" t="s">
+        <v>43</v>
       </c>
       <c r="H55" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I55" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J55"/>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
     </row>
     <row r="56" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="24">
+      <c r="A56" s="22">
         <v>63</v>
       </c>
-      <c r="B56" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D56" s="31" t="s">
-        <v>183</v>
-      </c>
-      <c r="E56" s="26"/>
-      <c r="F56" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="G56" s="28" t="s">
+      <c r="B56" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="E56" s="24"/>
+      <c r="F56" s="23" t="s">
         <v>179</v>
       </c>
+      <c r="G56" s="26" t="s">
+        <v>174</v>
+      </c>
       <c r="H56" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I56" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J56" s="20"/>
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
     </row>
     <row r="57" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="24">
+      <c r="A57" s="22">
         <v>64</v>
       </c>
-      <c r="B57" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C57" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D57" s="31" t="s">
-        <v>180</v>
-      </c>
-      <c r="E57" s="26"/>
-      <c r="F57" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="G57" s="28" t="s">
-        <v>37</v>
+      <c r="B57" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="E57" s="24"/>
+      <c r="F57" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="G57" s="26" t="s">
+        <v>36</v>
       </c>
       <c r="H57" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I57" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="J57" s="23" t="s">
-        <v>64</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="J57"/>
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
     </row>
     <row r="58" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="24">
+      <c r="A58" s="22">
         <v>65</v>
       </c>
-      <c r="B58" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C58" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D58" s="40" t="s">
-        <v>188</v>
-      </c>
-      <c r="E58" s="33"/>
-      <c r="F58" s="33" t="s">
-        <v>186</v>
-      </c>
-      <c r="G58" s="34"/>
+      <c r="B58" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" s="38" t="s">
+        <v>182</v>
+      </c>
+      <c r="E58" s="31"/>
+      <c r="F58" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="G58" s="32"/>
       <c r="H58" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="I58" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="J58" s="31"/>
+        <v>63</v>
+      </c>
+      <c r="I58" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="J58" s="29"/>
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
     </row>
     <row r="59" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="24">
+      <c r="A59" s="22">
         <v>66</v>
       </c>
-      <c r="B59" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="C59" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="D59" s="39" t="s">
-        <v>187</v>
-      </c>
-      <c r="E59" s="37"/>
-      <c r="F59" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="G59" s="28" t="s">
-        <v>189</v>
+      <c r="B59" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="E59" s="35"/>
+      <c r="F59" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="G59" s="26" t="s">
+        <v>183</v>
       </c>
       <c r="H59" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="I59" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="J59" s="38"/>
+        <v>64</v>
+      </c>
+      <c r="I59" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="J59" s="36"/>
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
     </row>
     <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G60" s="29"/>
+      <c r="G60" s="27"/>
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
       <c r="J60" s="6"/>
@@ -3481,7 +3480,7 @@
       <c r="L60" s="5"/>
     </row>
     <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G61" s="29"/>
+      <c r="G61" s="27"/>
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
       <c r="J61" s="6"/>
@@ -3489,7 +3488,7 @@
       <c r="L61" s="5"/>
     </row>
     <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G62" s="29"/>
+      <c r="G62" s="27"/>
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
       <c r="J62" s="6"/>
@@ -3497,7 +3496,7 @@
       <c r="L62" s="5"/>
     </row>
     <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G63" s="29"/>
+      <c r="G63" s="27"/>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
       <c r="J63" s="6"/>
@@ -3505,135 +3504,136 @@
       <c r="L63" s="5"/>
     </row>
     <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G64" s="29"/>
+      <c r="G64" s="27"/>
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
       <c r="J64" s="6"/>
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
     </row>
-    <row r="65" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G65" s="29"/>
+    <row r="65" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G65" s="27"/>
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
       <c r="J65" s="6"/>
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
     </row>
-    <row r="66" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G66" s="29"/>
+    <row r="66" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G66" s="27"/>
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
       <c r="J66" s="6"/>
       <c r="K66" s="5"/>
       <c r="L66" s="5"/>
     </row>
-    <row r="67" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G67" s="29"/>
+    <row r="67" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G67" s="27"/>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
       <c r="J67" s="6"/>
       <c r="K67" s="5"/>
       <c r="L67" s="5"/>
     </row>
-    <row r="68" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G68" s="29"/>
+    <row r="68" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G68" s="27"/>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
       <c r="J68" s="6"/>
       <c r="K68" s="5"/>
       <c r="L68" s="5"/>
     </row>
-    <row r="69" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G69" s="29"/>
+    <row r="69" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D69" s="40"/>
+      <c r="G69" s="27"/>
       <c r="H69" s="5"/>
       <c r="I69" s="5"/>
       <c r="J69" s="6"/>
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
     </row>
-    <row r="70" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G70" s="29"/>
+    <row r="70" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G70" s="27"/>
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
       <c r="J70" s="6"/>
       <c r="K70" s="5"/>
       <c r="L70" s="5"/>
     </row>
-    <row r="71" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G71" s="29"/>
+    <row r="71" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G71" s="27"/>
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
       <c r="J71" s="6"/>
       <c r="K71" s="5"/>
       <c r="L71" s="5"/>
     </row>
-    <row r="72" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G72" s="29"/>
+    <row r="72" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G72" s="27"/>
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
       <c r="J72" s="6"/>
       <c r="K72" s="5"/>
       <c r="L72" s="5"/>
     </row>
-    <row r="73" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G73" s="29"/>
+    <row r="73" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G73" s="27"/>
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>
       <c r="J73" s="6"/>
       <c r="K73" s="5"/>
       <c r="L73" s="5"/>
     </row>
-    <row r="74" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G74" s="29"/>
+    <row r="74" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G74" s="27"/>
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
       <c r="J74" s="6"/>
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
     </row>
-    <row r="75" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G75" s="29"/>
+    <row r="75" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G75" s="27"/>
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
       <c r="J75" s="6"/>
       <c r="K75" s="5"/>
       <c r="L75" s="5"/>
     </row>
-    <row r="76" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G76" s="29"/>
+    <row r="76" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G76" s="27"/>
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
       <c r="J76" s="6"/>
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
     </row>
-    <row r="77" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G77" s="29"/>
+    <row r="77" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G77" s="27"/>
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
       <c r="J77" s="6"/>
       <c r="K77" s="5"/>
       <c r="L77" s="5"/>
     </row>
-    <row r="78" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G78" s="29"/>
+    <row r="78" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G78" s="27"/>
       <c r="H78" s="5"/>
       <c r="I78" s="5"/>
       <c r="J78" s="6"/>
       <c r="K78" s="5"/>
       <c r="L78" s="5"/>
     </row>
-    <row r="79" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G79" s="29"/>
+    <row r="79" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G79" s="27"/>
       <c r="H79" s="5"/>
       <c r="I79" s="5"/>
       <c r="J79" s="6"/>
       <c r="K79" s="5"/>
       <c r="L79" s="5"/>
     </row>
-    <row r="80" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G80" s="29"/>
+    <row r="80" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G80" s="27"/>
       <c r="H80" s="5"/>
       <c r="I80" s="5"/>
       <c r="J80" s="6"/>
@@ -3641,7 +3641,7 @@
       <c r="L80" s="5"/>
     </row>
     <row r="81" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G81" s="29"/>
+      <c r="G81" s="27"/>
       <c r="H81" s="5"/>
       <c r="I81" s="5"/>
       <c r="J81" s="6"/>
@@ -3649,7 +3649,7 @@
       <c r="L81" s="5"/>
     </row>
     <row r="82" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G82" s="29"/>
+      <c r="G82" s="27"/>
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
       <c r="J82" s="6"/>
@@ -3657,7 +3657,7 @@
       <c r="L82" s="5"/>
     </row>
     <row r="83" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G83" s="29"/>
+      <c r="G83" s="27"/>
       <c r="H83" s="5"/>
       <c r="I83" s="5"/>
       <c r="J83" s="6"/>
@@ -3665,7 +3665,7 @@
       <c r="L83" s="5"/>
     </row>
     <row r="84" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G84" s="29"/>
+      <c r="G84" s="27"/>
       <c r="H84" s="5"/>
       <c r="I84" s="5"/>
       <c r="J84" s="6"/>
@@ -3673,7 +3673,7 @@
       <c r="L84" s="5"/>
     </row>
     <row r="85" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G85" s="29"/>
+      <c r="G85" s="27"/>
       <c r="H85" s="5"/>
       <c r="I85" s="5"/>
       <c r="J85" s="6"/>
@@ -3681,7 +3681,7 @@
       <c r="L85" s="5"/>
     </row>
     <row r="86" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G86" s="29"/>
+      <c r="G86" s="27"/>
       <c r="H86" s="5"/>
       <c r="I86" s="5"/>
       <c r="J86" s="6"/>
@@ -3689,7 +3689,7 @@
       <c r="L86" s="5"/>
     </row>
     <row r="87" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G87" s="29"/>
+      <c r="G87" s="27"/>
       <c r="H87" s="5"/>
       <c r="I87" s="5"/>
       <c r="J87" s="6"/>
@@ -3697,7 +3697,7 @@
       <c r="L87" s="5"/>
     </row>
     <row r="88" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G88" s="29"/>
+      <c r="G88" s="27"/>
       <c r="H88" s="5"/>
       <c r="I88" s="5"/>
       <c r="J88" s="6"/>
@@ -3705,7 +3705,7 @@
       <c r="L88" s="5"/>
     </row>
     <row r="89" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G89" s="29"/>
+      <c r="G89" s="27"/>
       <c r="H89" s="5"/>
       <c r="I89" s="5"/>
       <c r="J89" s="6"/>
@@ -3713,7 +3713,7 @@
       <c r="L89" s="5"/>
     </row>
     <row r="90" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G90" s="29"/>
+      <c r="G90" s="27"/>
       <c r="H90" s="5"/>
       <c r="I90" s="5"/>
       <c r="J90" s="6"/>
@@ -3721,7 +3721,7 @@
       <c r="L90" s="5"/>
     </row>
     <row r="91" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G91" s="29"/>
+      <c r="G91" s="27"/>
       <c r="H91" s="5"/>
       <c r="I91" s="5"/>
       <c r="J91" s="6"/>
@@ -3729,7 +3729,7 @@
       <c r="L91" s="5"/>
     </row>
     <row r="92" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G92" s="29"/>
+      <c r="G92" s="27"/>
       <c r="H92" s="5"/>
       <c r="I92" s="5"/>
       <c r="J92" s="6"/>
@@ -3737,7 +3737,7 @@
       <c r="L92" s="5"/>
     </row>
     <row r="93" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G93" s="29"/>
+      <c r="G93" s="27"/>
       <c r="H93" s="5"/>
       <c r="I93" s="5"/>
       <c r="J93" s="6"/>
@@ -3745,7 +3745,7 @@
       <c r="L93" s="5"/>
     </row>
     <row r="94" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G94" s="29"/>
+      <c r="G94" s="27"/>
       <c r="H94" s="5"/>
       <c r="I94" s="5"/>
       <c r="J94" s="6"/>
@@ -3753,7 +3753,7 @@
       <c r="L94" s="5"/>
     </row>
     <row r="95" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G95" s="29"/>
+      <c r="G95" s="27"/>
       <c r="H95" s="5"/>
       <c r="I95" s="5"/>
       <c r="J95" s="6"/>
@@ -3761,7 +3761,7 @@
       <c r="L95" s="5"/>
     </row>
     <row r="96" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G96" s="29"/>
+      <c r="G96" s="27"/>
       <c r="H96" s="5"/>
       <c r="I96" s="5"/>
       <c r="J96" s="6"/>
@@ -3769,7 +3769,7 @@
       <c r="L96" s="5"/>
     </row>
     <row r="97" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G97" s="29"/>
+      <c r="G97" s="27"/>
       <c r="H97" s="5"/>
       <c r="I97" s="5"/>
       <c r="J97" s="6"/>
@@ -3777,7 +3777,7 @@
       <c r="L97" s="5"/>
     </row>
     <row r="98" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G98" s="29"/>
+      <c r="G98" s="27"/>
       <c r="H98" s="5"/>
       <c r="I98" s="5"/>
       <c r="J98" s="6"/>
@@ -3785,7 +3785,7 @@
       <c r="L98" s="5"/>
     </row>
     <row r="99" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G99" s="29"/>
+      <c r="G99" s="27"/>
       <c r="H99" s="5"/>
       <c r="I99" s="5"/>
       <c r="J99" s="6"/>
@@ -3793,7 +3793,7 @@
       <c r="L99" s="5"/>
     </row>
     <row r="100" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G100" s="29"/>
+      <c r="G100" s="27"/>
       <c r="H100" s="5"/>
       <c r="I100" s="5"/>
       <c r="J100" s="6"/>
@@ -3801,7 +3801,7 @@
       <c r="L100" s="5"/>
     </row>
     <row r="101" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G101" s="29"/>
+      <c r="G101" s="27"/>
       <c r="H101" s="5"/>
       <c r="I101" s="5"/>
       <c r="J101" s="6"/>
@@ -3809,7 +3809,7 @@
       <c r="L101" s="5"/>
     </row>
     <row r="102" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G102" s="29"/>
+      <c r="G102" s="27"/>
       <c r="H102" s="5"/>
       <c r="I102" s="5"/>
       <c r="J102" s="6"/>
@@ -3817,7 +3817,7 @@
       <c r="L102" s="5"/>
     </row>
     <row r="103" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G103" s="29"/>
+      <c r="G103" s="27"/>
       <c r="H103" s="5"/>
       <c r="I103" s="5"/>
       <c r="J103" s="6"/>
@@ -3825,7 +3825,7 @@
       <c r="L103" s="5"/>
     </row>
     <row r="104" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G104" s="29"/>
+      <c r="G104" s="27"/>
       <c r="H104" s="5"/>
       <c r="I104" s="5"/>
       <c r="J104" s="6"/>
@@ -3833,7 +3833,7 @@
       <c r="L104" s="5"/>
     </row>
     <row r="105" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G105" s="29"/>
+      <c r="G105" s="27"/>
       <c r="H105" s="5"/>
       <c r="I105" s="5"/>
       <c r="J105" s="6"/>
@@ -3841,7 +3841,7 @@
       <c r="L105" s="5"/>
     </row>
     <row r="106" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G106" s="29"/>
+      <c r="G106" s="27"/>
       <c r="H106" s="5"/>
       <c r="I106" s="5"/>
       <c r="J106" s="6"/>
@@ -3849,7 +3849,7 @@
       <c r="L106" s="5"/>
     </row>
     <row r="107" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G107" s="29"/>
+      <c r="G107" s="27"/>
       <c r="H107" s="5"/>
       <c r="I107" s="5"/>
       <c r="J107" s="6"/>
@@ -3857,7 +3857,7 @@
       <c r="L107" s="5"/>
     </row>
     <row r="108" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G108" s="29"/>
+      <c r="G108" s="27"/>
       <c r="H108" s="5"/>
       <c r="I108" s="5"/>
       <c r="J108" s="6"/>
@@ -3865,7 +3865,7 @@
       <c r="L108" s="5"/>
     </row>
     <row r="109" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G109" s="29"/>
+      <c r="G109" s="27"/>
       <c r="H109" s="5"/>
       <c r="I109" s="5"/>
       <c r="J109" s="6"/>
@@ -3873,7 +3873,7 @@
       <c r="L109" s="5"/>
     </row>
     <row r="110" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G110" s="29"/>
+      <c r="G110" s="27"/>
       <c r="H110" s="5"/>
       <c r="I110" s="5"/>
       <c r="J110" s="6"/>
@@ -3881,7 +3881,7 @@
       <c r="L110" s="5"/>
     </row>
     <row r="111" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G111" s="29"/>
+      <c r="G111" s="27"/>
       <c r="H111" s="5"/>
       <c r="I111" s="5"/>
       <c r="J111" s="6"/>
@@ -3889,7 +3889,7 @@
       <c r="L111" s="5"/>
     </row>
     <row r="112" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G112" s="29"/>
+      <c r="G112" s="27"/>
       <c r="H112" s="5"/>
       <c r="I112" s="5"/>
       <c r="J112" s="6"/>
@@ -3897,7 +3897,7 @@
       <c r="L112" s="5"/>
     </row>
     <row r="113" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G113" s="29"/>
+      <c r="G113" s="27"/>
       <c r="H113" s="5"/>
       <c r="I113" s="5"/>
       <c r="J113" s="6"/>
@@ -3905,7 +3905,7 @@
       <c r="L113" s="5"/>
     </row>
     <row r="114" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G114" s="29"/>
+      <c r="G114" s="27"/>
       <c r="H114" s="5"/>
       <c r="I114" s="5"/>
       <c r="J114" s="6"/>
@@ -3913,7 +3913,7 @@
       <c r="L114" s="5"/>
     </row>
     <row r="115" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G115" s="29"/>
+      <c r="G115" s="27"/>
       <c r="H115" s="5"/>
       <c r="I115" s="5"/>
       <c r="J115" s="6"/>
@@ -3921,7 +3921,7 @@
       <c r="L115" s="5"/>
     </row>
     <row r="116" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G116" s="29"/>
+      <c r="G116" s="27"/>
       <c r="H116" s="5"/>
       <c r="I116" s="5"/>
       <c r="J116" s="6"/>
@@ -3929,7 +3929,7 @@
       <c r="L116" s="5"/>
     </row>
     <row r="117" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G117" s="29"/>
+      <c r="G117" s="27"/>
       <c r="H117" s="5"/>
       <c r="I117" s="5"/>
       <c r="J117" s="6"/>
@@ -3937,7 +3937,7 @@
       <c r="L117" s="5"/>
     </row>
     <row r="118" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G118" s="29"/>
+      <c r="G118" s="27"/>
       <c r="H118" s="5"/>
       <c r="I118" s="5"/>
       <c r="J118" s="6"/>
@@ -3945,7 +3945,7 @@
       <c r="L118" s="5"/>
     </row>
     <row r="119" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G119" s="29"/>
+      <c r="G119" s="27"/>
       <c r="H119" s="5"/>
       <c r="I119" s="5"/>
       <c r="J119" s="6"/>
@@ -3953,7 +3953,7 @@
       <c r="L119" s="5"/>
     </row>
     <row r="120" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G120" s="29"/>
+      <c r="G120" s="27"/>
       <c r="H120" s="5"/>
       <c r="I120" s="5"/>
       <c r="J120" s="6"/>
@@ -3961,7 +3961,7 @@
       <c r="L120" s="5"/>
     </row>
     <row r="121" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G121" s="29"/>
+      <c r="G121" s="27"/>
       <c r="H121" s="5"/>
       <c r="I121" s="5"/>
       <c r="J121" s="6"/>
@@ -3969,7 +3969,7 @@
       <c r="L121" s="5"/>
     </row>
     <row r="122" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G122" s="29"/>
+      <c r="G122" s="27"/>
       <c r="H122" s="5"/>
       <c r="I122" s="5"/>
       <c r="J122" s="6"/>
@@ -3977,7 +3977,7 @@
       <c r="L122" s="5"/>
     </row>
     <row r="123" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G123" s="29"/>
+      <c r="G123" s="27"/>
       <c r="H123" s="5"/>
       <c r="I123" s="5"/>
       <c r="J123" s="6"/>
@@ -3985,7 +3985,7 @@
       <c r="L123" s="5"/>
     </row>
     <row r="124" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G124" s="29"/>
+      <c r="G124" s="27"/>
       <c r="H124" s="5"/>
       <c r="I124" s="5"/>
       <c r="J124" s="6"/>
@@ -3993,7 +3993,7 @@
       <c r="L124" s="5"/>
     </row>
     <row r="125" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G125" s="29"/>
+      <c r="G125" s="27"/>
       <c r="H125" s="5"/>
       <c r="I125" s="5"/>
       <c r="J125" s="6"/>
@@ -4001,7 +4001,7 @@
       <c r="L125" s="5"/>
     </row>
     <row r="126" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G126" s="29"/>
+      <c r="G126" s="27"/>
       <c r="H126" s="5"/>
       <c r="I126" s="5"/>
       <c r="J126" s="6"/>
@@ -4009,7 +4009,7 @@
       <c r="L126" s="5"/>
     </row>
     <row r="127" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G127" s="29"/>
+      <c r="G127" s="27"/>
       <c r="H127" s="5"/>
       <c r="I127" s="5"/>
       <c r="J127" s="6"/>
@@ -4017,7 +4017,7 @@
       <c r="L127" s="5"/>
     </row>
     <row r="128" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G128" s="29"/>
+      <c r="G128" s="27"/>
       <c r="H128" s="5"/>
       <c r="I128" s="5"/>
       <c r="J128" s="6"/>
@@ -4025,7 +4025,7 @@
       <c r="L128" s="5"/>
     </row>
     <row r="129" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G129" s="29"/>
+      <c r="G129" s="27"/>
       <c r="H129" s="5"/>
       <c r="I129" s="5"/>
       <c r="J129" s="6"/>
@@ -4033,7 +4033,7 @@
       <c r="L129" s="5"/>
     </row>
     <row r="130" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G130" s="29"/>
+      <c r="G130" s="27"/>
       <c r="H130" s="5"/>
       <c r="I130" s="5"/>
       <c r="J130" s="6"/>
@@ -4041,7 +4041,7 @@
       <c r="L130" s="5"/>
     </row>
     <row r="131" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G131" s="29"/>
+      <c r="G131" s="27"/>
       <c r="H131" s="5"/>
       <c r="I131" s="5"/>
       <c r="J131" s="6"/>
@@ -4049,7 +4049,7 @@
       <c r="L131" s="5"/>
     </row>
     <row r="132" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G132" s="29"/>
+      <c r="G132" s="27"/>
       <c r="H132" s="5"/>
       <c r="I132" s="5"/>
       <c r="J132" s="6"/>
@@ -4057,7 +4057,7 @@
       <c r="L132" s="5"/>
     </row>
     <row r="133" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G133" s="29"/>
+      <c r="G133" s="27"/>
       <c r="H133" s="5"/>
       <c r="I133" s="5"/>
       <c r="J133" s="6"/>
@@ -4065,7 +4065,7 @@
       <c r="L133" s="5"/>
     </row>
     <row r="134" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G134" s="29"/>
+      <c r="G134" s="27"/>
       <c r="H134" s="5"/>
       <c r="I134" s="5"/>
       <c r="J134" s="6"/>
@@ -4073,7 +4073,7 @@
       <c r="L134" s="5"/>
     </row>
     <row r="135" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G135" s="29"/>
+      <c r="G135" s="27"/>
       <c r="H135" s="5"/>
       <c r="I135" s="5"/>
       <c r="J135" s="6"/>
@@ -4081,7 +4081,7 @@
       <c r="L135" s="5"/>
     </row>
     <row r="136" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G136" s="29"/>
+      <c r="G136" s="27"/>
       <c r="H136" s="5"/>
       <c r="I136" s="5"/>
       <c r="J136" s="6"/>
@@ -4089,7 +4089,7 @@
       <c r="L136" s="5"/>
     </row>
     <row r="137" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G137" s="29"/>
+      <c r="G137" s="27"/>
       <c r="H137" s="5"/>
       <c r="I137" s="5"/>
       <c r="J137" s="6"/>
@@ -4097,7 +4097,7 @@
       <c r="L137" s="5"/>
     </row>
     <row r="138" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G138" s="29"/>
+      <c r="G138" s="27"/>
       <c r="H138" s="5"/>
       <c r="I138" s="5"/>
       <c r="J138" s="6"/>
@@ -4105,7 +4105,7 @@
       <c r="L138" s="5"/>
     </row>
     <row r="139" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G139" s="29"/>
+      <c r="G139" s="27"/>
       <c r="H139" s="5"/>
       <c r="I139" s="5"/>
       <c r="J139" s="6"/>
@@ -4113,7 +4113,7 @@
       <c r="L139" s="5"/>
     </row>
     <row r="140" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G140" s="29"/>
+      <c r="G140" s="27"/>
       <c r="H140" s="5"/>
       <c r="I140" s="5"/>
       <c r="J140" s="6"/>
@@ -4121,7 +4121,7 @@
       <c r="L140" s="5"/>
     </row>
     <row r="141" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G141" s="29"/>
+      <c r="G141" s="27"/>
       <c r="H141" s="5"/>
       <c r="I141" s="5"/>
       <c r="J141" s="6"/>
@@ -4129,7 +4129,7 @@
       <c r="L141" s="5"/>
     </row>
     <row r="142" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G142" s="29"/>
+      <c r="G142" s="27"/>
       <c r="H142" s="5"/>
       <c r="I142" s="5"/>
       <c r="J142" s="6"/>
@@ -4137,7 +4137,7 @@
       <c r="L142" s="5"/>
     </row>
     <row r="143" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G143" s="29"/>
+      <c r="G143" s="27"/>
       <c r="H143" s="5"/>
       <c r="I143" s="5"/>
       <c r="J143" s="6"/>
@@ -4145,7 +4145,7 @@
       <c r="L143" s="5"/>
     </row>
     <row r="144" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G144" s="29"/>
+      <c r="G144" s="27"/>
       <c r="H144" s="5"/>
       <c r="I144" s="5"/>
       <c r="J144" s="6"/>
@@ -4204,7 +4204,7 @@
   <conditionalFormatting sqref="G60:G1048576 G1:G52">
     <cfRule type="duplicateValues" dxfId="15" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D60:D1048576 D1">
+  <conditionalFormatting sqref="D60:D68 D1 D70:D1048576">
     <cfRule type="duplicateValues" dxfId="14" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">

</xml_diff>

<commit_message>
spring boot with mongo db: integration example added, eCommerce db with relationship added
</commit_message>
<xml_diff>
--- a/project/MRU Java FSD Project Final.xlsx
+++ b/project/MRU Java FSD Project Final.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="189">
   <si>
     <t xml:space="preserve">University </t>
   </si>
@@ -44,9 +44,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Remarks</t>
-  </si>
-  <si>
     <t>Malla Reddy University</t>
   </si>
   <si>
@@ -182,9 +179,6 @@
     <t>2211CS030017</t>
   </si>
   <si>
-    <t>2211CS0130085</t>
-  </si>
-  <si>
     <t>2211CS030164</t>
   </si>
   <si>
@@ -588,6 +582,15 @@
   </si>
   <si>
     <t>HOME COOK SERVICE MANAGEMENT</t>
+  </si>
+  <si>
+    <t>2211CS030085</t>
+  </si>
+  <si>
+    <t>Assignment 2 Review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registration Form is too simple, </t>
   </si>
 </sst>
 </file>
@@ -793,7 +796,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -852,9 +855,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -891,15 +891,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
@@ -909,8 +900,28 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1497,6 +1508,10 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:J59" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:J59"/>
+  <sortState ref="A2:J59">
+    <sortCondition ref="H2:H59"/>
+    <sortCondition ref="G2:G59"/>
+  </sortState>
   <tableColumns count="10">
     <tableColumn id="1" name="S.no" dataDxfId="9"/>
     <tableColumn id="2" name="University " dataDxfId="8"/>
@@ -1507,7 +1522,7 @@
     <tableColumn id="6" name="Team Leader Roll No" dataDxfId="3"/>
     <tableColumn id="7" name="Batch" dataDxfId="2"/>
     <tableColumn id="8" name="Status" dataDxfId="1"/>
-    <tableColumn id="9" name="Remarks" dataDxfId="0"/>
+    <tableColumn id="9" name="Assignment 2 Review" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1781,20 +1796,20 @@
   </sheetPr>
   <dimension ref="A1:L144"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G58" sqref="G58"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" style="29" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="63.109375" style="13" customWidth="1"/>
     <col min="5" max="5" width="23.77734375" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.88671875" style="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.88671875" style="27" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="66.6640625" style="2" customWidth="1"/>
@@ -1804,7 +1819,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -1816,22 +1831,22 @@
         <v>2</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="24" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>6</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1839,54 +1854,58 @@
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="E2" s="17"/>
+        <v>140</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>170</v>
+      </c>
       <c r="F2" s="15" t="s">
-        <v>9</v>
+        <v>87</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>10</v>
+        <v>169</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="20"/>
+        <v>11</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14">
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="E3" s="17"/>
       <c r="F3" s="15" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J3" s="20"/>
     </row>
@@ -1895,26 +1914,26 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E4" s="17"/>
       <c r="F4" s="15" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J4" s="20"/>
     </row>
@@ -1923,54 +1942,54 @@
         <v>4</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>126</v>
+        <v>168</v>
       </c>
       <c r="E5" s="17"/>
       <c r="F5" s="15" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>16</v>
+        <v>118</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="20"/>
+        <v>11</v>
+      </c>
+      <c r="J5" s="21"/>
     </row>
     <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14">
         <v>5</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="E6" s="17"/>
       <c r="F6" s="15" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J6" s="20"/>
     </row>
@@ -1979,26 +1998,26 @@
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="E7" s="17"/>
       <c r="F7" s="15" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J7" s="20"/>
     </row>
@@ -2007,26 +2026,26 @@
         <v>7</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="15" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J8" s="20"/>
     </row>
@@ -2035,26 +2054,26 @@
         <v>8</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="E9" s="17"/>
       <c r="F9" s="15" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J9" s="20"/>
     </row>
@@ -2063,26 +2082,26 @@
         <v>9</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E10" s="17"/>
       <c r="F10" s="15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J10" s="20"/>
     </row>
@@ -2091,1388 +2110,1386 @@
         <v>10</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="E11" s="17"/>
       <c r="F11" s="15" t="s">
-        <v>80</v>
+        <v>14</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J11" s="20"/>
     </row>
     <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="15" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J12" s="20"/>
     </row>
     <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
+        <v>12</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="E13" s="17"/>
+      <c r="F13" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="20"/>
+    </row>
+    <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="14">
         <v>13</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="E13" s="17"/>
-      <c r="F13" s="20" t="str">
+      <c r="B14" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="20"/>
+    </row>
+    <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="14">
+        <v>14</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="E15" s="17"/>
+      <c r="F15" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="20"/>
+    </row>
+    <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="14">
+        <v>15</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="E16" s="17"/>
+      <c r="F16" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="20"/>
+    </row>
+    <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="14">
+        <v>16</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="E17" s="17"/>
+      <c r="F17" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="20"/>
+    </row>
+    <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="14">
+        <v>17</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="E18" s="17"/>
+      <c r="F18" s="20" t="str">
         <f ca="1">UPPER(Form_Responses1[[#This Row],[Team Leader Name]])</f>
         <v>G.SAI KAVYA</v>
       </c>
-      <c r="G13" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="I13" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="J13" s="20"/>
-    </row>
-    <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="14">
-        <v>14</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="G14" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="I14" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="J14" s="20"/>
-    </row>
-    <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="14">
-        <v>15</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="I15" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="J15" s="20"/>
-    </row>
-    <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="14">
-        <v>16</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="G16" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="I16" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="J16" s="20"/>
-    </row>
-    <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14">
-        <v>17</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="G17" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="I17" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="J17" s="20"/>
-    </row>
-    <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="14">
-        <v>18</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="E18" s="17"/>
-      <c r="F18" s="15" t="s">
-        <v>84</v>
-      </c>
       <c r="G18" s="18" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J18" s="20"/>
     </row>
     <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="15" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J19" s="20"/>
     </row>
     <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J20" s="20"/>
     </row>
     <row r="21" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>170</v>
+        <v>131</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="15" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>120</v>
+        <v>27</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="J21" s="21"/>
+        <v>11</v>
+      </c>
+      <c r="J21" s="20"/>
     </row>
     <row r="22" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>172</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="E22" s="17"/>
       <c r="F22" s="15" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>171</v>
+        <v>23</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J22" s="20"/>
     </row>
     <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="15" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J23" s="20"/>
     </row>
     <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>144</v>
+        <v>121</v>
       </c>
       <c r="E24" s="17"/>
       <c r="F24" s="15" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J24" s="20"/>
     </row>
     <row r="25" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="14">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>51</v>
+        <v>186</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I25" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J25" s="20"/>
     </row>
     <row r="26" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="14">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="E26" s="17"/>
       <c r="F26" s="15" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I26" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J26" s="20"/>
     </row>
     <row r="27" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="14">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="E27" s="17"/>
       <c r="F27" s="15" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I27" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J27" s="20"/>
     </row>
     <row r="28" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="14">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="15" t="s">
-        <v>95</v>
+        <v>20</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J28" s="20"/>
     </row>
     <row r="29" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="14">
-        <v>32</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="E29" s="17"/>
-      <c r="F29" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="G29" s="18" t="s">
-        <v>17</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="37" t="s">
+        <v>180</v>
+      </c>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="G29" s="31"/>
       <c r="H29" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="I29" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="J29" s="20"/>
+        <v>61</v>
+      </c>
+      <c r="I29" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J29" s="28"/>
     </row>
     <row r="30" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="14">
-        <v>33</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="E30" s="17"/>
-      <c r="F30" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="G30" s="18" t="s">
-        <v>23</v>
+        <v>29</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="E30" s="23"/>
+      <c r="F30" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="G30" s="25" t="s">
+        <v>41</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I30" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="14">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>122</v>
+        <v>151</v>
       </c>
       <c r="E31" s="17"/>
       <c r="F31" s="15" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="G31" s="18" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I31" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="J31" s="21"/>
+        <v>11</v>
+      </c>
+      <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="14">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E32" s="17"/>
       <c r="F32" s="15" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G32" s="18" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I32" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J32" s="20"/>
     </row>
     <row r="33" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="14">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E33" s="17"/>
       <c r="F33" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G33" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I33" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J33" s="20"/>
     </row>
     <row r="34" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="14">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="E34" s="17"/>
       <c r="F34" s="15" t="s">
-        <v>38</v>
+        <v>113</v>
       </c>
       <c r="G34" s="18" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I34" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J34" s="20"/>
     </row>
     <row r="35" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="14">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>187</v>
+        <v>120</v>
       </c>
       <c r="E35" s="17"/>
       <c r="F35" s="15" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I35" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="J35"/>
+        <v>11</v>
+      </c>
+      <c r="J35" s="45"/>
     </row>
     <row r="36" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="14">
-        <v>41</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="E36" s="17"/>
-      <c r="F36" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="G36" s="18" t="s">
-        <v>45</v>
+        <v>35</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="G36" s="25" t="s">
+        <v>181</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="I36" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="J36" s="20"/>
+        <v>62</v>
+      </c>
+      <c r="I36" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="J36" s="28"/>
     </row>
     <row r="37" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="14">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="E37" s="17"/>
       <c r="F37" s="15" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="G37" s="18" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H37" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J37" s="20"/>
     </row>
     <row r="38" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="14">
-        <v>44</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="E38" s="17"/>
-      <c r="F38" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="G38" s="18" t="s">
-        <v>50</v>
+        <v>37</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="39" t="s">
+        <v>184</v>
+      </c>
+      <c r="E38" s="23"/>
+      <c r="F38" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I38" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="J38" s="20"/>
+        <v>11</v>
+      </c>
+      <c r="J38" s="42"/>
     </row>
     <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="14">
+        <v>38</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="E39" s="23"/>
+      <c r="F39" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="G39" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="E39" s="17"/>
-      <c r="F39" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="G39" s="18" t="s">
-        <v>69</v>
-      </c>
       <c r="H39" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I39" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J39" s="20"/>
     </row>
     <row r="40" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="14">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="E40" s="17"/>
       <c r="F40" s="15" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G40" s="18" t="s">
         <v>70</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I40" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J40" s="20"/>
     </row>
     <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="14">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D41" s="38" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
       <c r="E41" s="17"/>
       <c r="F41" s="15" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="G41" s="18" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I41" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="J41"/>
+        <v>11</v>
+      </c>
+      <c r="J41" s="43"/>
     </row>
     <row r="42" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="14">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E42" s="17"/>
       <c r="F42" s="15" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G42" s="18" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="H42" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I42" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J42" s="20"/>
     </row>
     <row r="43" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="14">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="E43" s="17"/>
       <c r="F43" s="15" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="G43" s="18" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="H43" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I43" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J43" s="20"/>
     </row>
     <row r="44" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="14">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="E44" s="17"/>
       <c r="F44" s="15" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G44" s="18" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H44" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I44" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J44" s="20"/>
     </row>
     <row r="45" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="14">
-        <v>51</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D45" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="E45" s="17"/>
-      <c r="F45" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="G45" s="18" t="s">
-        <v>73</v>
+        <v>44</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="E45" s="23"/>
+      <c r="F45" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="G45" s="25" t="s">
+        <v>172</v>
       </c>
       <c r="H45" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I45" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J45" s="20"/>
     </row>
     <row r="46" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A46" s="14">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E46" s="17"/>
       <c r="F46" s="15" t="s">
-        <v>113</v>
+        <v>56</v>
       </c>
       <c r="G46" s="18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H46" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I46" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J46" s="20"/>
     </row>
     <row r="47" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="14">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="E47" s="17"/>
       <c r="F47" s="15" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="G47" s="18" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="H47" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I47" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J47" s="20"/>
     </row>
     <row r="48" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="14">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E48" s="17"/>
       <c r="F48" s="15" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="G48" s="18" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="H48" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I48" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J48" s="20"/>
     </row>
     <row r="49" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="14">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="E49" s="17"/>
       <c r="F49" s="15" t="s">
-        <v>58</v>
+        <v>97</v>
       </c>
       <c r="G49" s="18" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I49" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J49" s="20"/>
     </row>
     <row r="50" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="14">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="E50" s="17"/>
       <c r="F50" s="15" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="G50" s="18" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="H50" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I50" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J50" s="20"/>
     </row>
     <row r="51" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="14">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C51" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D51" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="E51" s="17"/>
+        <v>7</v>
+      </c>
+      <c r="D51" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="E51" s="19"/>
       <c r="F51" s="15" t="s">
         <v>117</v>
       </c>
       <c r="G51" s="18" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="H51" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I51" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J51" s="20"/>
     </row>
     <row r="52" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="14">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D52" s="20" t="s">
-        <v>168</v>
-      </c>
-      <c r="E52" s="19"/>
+        <v>7</v>
+      </c>
+      <c r="D52" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="E52" s="17"/>
       <c r="F52" s="15" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="G52" s="18" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="H52" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I52" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J52" s="20"/>
     </row>
     <row r="53" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="22">
-        <v>60</v>
-      </c>
-      <c r="B53" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D53" s="23" t="s">
-        <v>175</v>
-      </c>
-      <c r="E53" s="24"/>
-      <c r="F53" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="G53" s="26" t="s">
-        <v>42</v>
+      <c r="A53" s="14">
+        <v>52</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="E53" s="17"/>
+      <c r="F53" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="G53" s="18" t="s">
+        <v>43</v>
       </c>
       <c r="H53" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I53" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="J53" s="20"/>
+        <v>11</v>
+      </c>
+      <c r="J53" s="42"/>
     </row>
     <row r="54" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="22">
-        <v>61</v>
-      </c>
-      <c r="B54" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C54" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D54" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="E54" s="24"/>
-      <c r="F54" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="G54" s="26" t="s">
-        <v>46</v>
+      <c r="A54" s="14">
+        <v>53</v>
+      </c>
+      <c r="B54" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="E54" s="17"/>
+      <c r="F54" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="G54" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="H54" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I54" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J54" s="20"/>
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
     </row>
     <row r="55" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="22">
+      <c r="A55" s="14">
+        <v>54</v>
+      </c>
+      <c r="B55" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="E55" s="17"/>
+      <c r="F55" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="G55" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="H55" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B55" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D55" s="39" t="s">
-        <v>184</v>
-      </c>
-      <c r="E55" s="24"/>
-      <c r="F55" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="G55" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="H55" s="15" t="s">
-        <v>64</v>
-      </c>
       <c r="I55" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J55"/>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
     </row>
     <row r="56" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="22">
-        <v>63</v>
-      </c>
-      <c r="B56" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D56" s="29" t="s">
-        <v>177</v>
-      </c>
-      <c r="E56" s="24"/>
-      <c r="F56" s="23" t="s">
-        <v>179</v>
-      </c>
-      <c r="G56" s="26" t="s">
-        <v>174</v>
+      <c r="A56" s="14">
+        <v>55</v>
+      </c>
+      <c r="B56" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="E56" s="17"/>
+      <c r="F56" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="G56" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="H56" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I56" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J56" s="20"/>
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
     </row>
     <row r="57" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="22">
-        <v>64</v>
-      </c>
-      <c r="B57" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C57" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D57" s="41" t="s">
-        <v>186</v>
-      </c>
-      <c r="E57" s="24"/>
-      <c r="F57" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="G57" s="26" t="s">
-        <v>36</v>
+      <c r="A57" s="14">
+        <v>56</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" s="38" t="s">
+        <v>159</v>
+      </c>
+      <c r="E57" s="17"/>
+      <c r="F57" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="G57" s="18" t="s">
+        <v>71</v>
       </c>
       <c r="H57" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I57" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="J57"/>
+        <v>11</v>
+      </c>
+      <c r="J57" s="43"/>
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
     </row>
     <row r="58" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="22">
-        <v>65</v>
-      </c>
-      <c r="B58" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C58" s="26" t="s">
-        <v>8</v>
+      <c r="A58" s="14">
+        <v>57</v>
+      </c>
+      <c r="B58" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>7</v>
       </c>
       <c r="D58" s="38" t="s">
-        <v>182</v>
-      </c>
-      <c r="E58" s="31"/>
-      <c r="F58" s="31" t="s">
-        <v>180</v>
-      </c>
-      <c r="G58" s="32"/>
+        <v>154</v>
+      </c>
+      <c r="E58" s="17"/>
+      <c r="F58" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="G58" s="18" t="s">
+        <v>49</v>
+      </c>
       <c r="H58" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="I58" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="J58" s="29"/>
+        <v>62</v>
+      </c>
+      <c r="I58" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J58" s="20"/>
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
     </row>
     <row r="59" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="22">
-        <v>66</v>
-      </c>
-      <c r="B59" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="C59" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="D59" s="37" t="s">
-        <v>181</v>
-      </c>
-      <c r="E59" s="35"/>
-      <c r="F59" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="G59" s="26" t="s">
-        <v>183</v>
+      <c r="A59" s="14">
+        <v>58</v>
+      </c>
+      <c r="B59" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="E59" s="41"/>
+      <c r="F59" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="G59" s="25" t="s">
+        <v>42</v>
       </c>
       <c r="H59" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="I59" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="J59" s="36"/>
+        <v>62</v>
+      </c>
+      <c r="I59" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J59" s="44"/>
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
     </row>
     <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G60" s="27"/>
+      <c r="G60" s="26"/>
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
       <c r="J60" s="6"/>
@@ -3480,7 +3497,7 @@
       <c r="L60" s="5"/>
     </row>
     <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G61" s="27"/>
+      <c r="G61" s="26"/>
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
       <c r="J61" s="6"/>
@@ -3488,7 +3505,7 @@
       <c r="L61" s="5"/>
     </row>
     <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G62" s="27"/>
+      <c r="G62" s="26"/>
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
       <c r="J62" s="6"/>
@@ -3496,7 +3513,7 @@
       <c r="L62" s="5"/>
     </row>
     <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G63" s="27"/>
+      <c r="G63" s="26"/>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
       <c r="J63" s="6"/>
@@ -3504,7 +3521,7 @@
       <c r="L63" s="5"/>
     </row>
     <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G64" s="27"/>
+      <c r="G64" s="26"/>
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
       <c r="J64" s="6"/>
@@ -3512,7 +3529,7 @@
       <c r="L64" s="5"/>
     </row>
     <row r="65" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G65" s="27"/>
+      <c r="G65" s="26"/>
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
       <c r="J65" s="6"/>
@@ -3520,7 +3537,7 @@
       <c r="L65" s="5"/>
     </row>
     <row r="66" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G66" s="27"/>
+      <c r="G66" s="26"/>
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
       <c r="J66" s="6"/>
@@ -3528,7 +3545,7 @@
       <c r="L66" s="5"/>
     </row>
     <row r="67" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G67" s="27"/>
+      <c r="G67" s="26"/>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
       <c r="J67" s="6"/>
@@ -3536,7 +3553,7 @@
       <c r="L67" s="5"/>
     </row>
     <row r="68" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G68" s="27"/>
+      <c r="G68" s="26"/>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
       <c r="J68" s="6"/>
@@ -3544,8 +3561,8 @@
       <c r="L68" s="5"/>
     </row>
     <row r="69" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D69" s="40"/>
-      <c r="G69" s="27"/>
+      <c r="D69" s="36"/>
+      <c r="G69" s="26"/>
       <c r="H69" s="5"/>
       <c r="I69" s="5"/>
       <c r="J69" s="6"/>
@@ -3553,7 +3570,7 @@
       <c r="L69" s="5"/>
     </row>
     <row r="70" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G70" s="27"/>
+      <c r="G70" s="26"/>
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
       <c r="J70" s="6"/>
@@ -3561,7 +3578,7 @@
       <c r="L70" s="5"/>
     </row>
     <row r="71" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G71" s="27"/>
+      <c r="G71" s="26"/>
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
       <c r="J71" s="6"/>
@@ -3569,7 +3586,7 @@
       <c r="L71" s="5"/>
     </row>
     <row r="72" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G72" s="27"/>
+      <c r="G72" s="26"/>
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
       <c r="J72" s="6"/>
@@ -3577,7 +3594,7 @@
       <c r="L72" s="5"/>
     </row>
     <row r="73" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G73" s="27"/>
+      <c r="G73" s="26"/>
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>
       <c r="J73" s="6"/>
@@ -3585,7 +3602,7 @@
       <c r="L73" s="5"/>
     </row>
     <row r="74" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G74" s="27"/>
+      <c r="G74" s="26"/>
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
       <c r="J74" s="6"/>
@@ -3593,7 +3610,7 @@
       <c r="L74" s="5"/>
     </row>
     <row r="75" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G75" s="27"/>
+      <c r="G75" s="26"/>
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
       <c r="J75" s="6"/>
@@ -3601,7 +3618,7 @@
       <c r="L75" s="5"/>
     </row>
     <row r="76" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G76" s="27"/>
+      <c r="G76" s="26"/>
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
       <c r="J76" s="6"/>
@@ -3609,7 +3626,7 @@
       <c r="L76" s="5"/>
     </row>
     <row r="77" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G77" s="27"/>
+      <c r="G77" s="26"/>
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
       <c r="J77" s="6"/>
@@ -3617,7 +3634,7 @@
       <c r="L77" s="5"/>
     </row>
     <row r="78" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G78" s="27"/>
+      <c r="G78" s="26"/>
       <c r="H78" s="5"/>
       <c r="I78" s="5"/>
       <c r="J78" s="6"/>
@@ -3625,7 +3642,7 @@
       <c r="L78" s="5"/>
     </row>
     <row r="79" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G79" s="27"/>
+      <c r="G79" s="26"/>
       <c r="H79" s="5"/>
       <c r="I79" s="5"/>
       <c r="J79" s="6"/>
@@ -3633,7 +3650,7 @@
       <c r="L79" s="5"/>
     </row>
     <row r="80" spans="4:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G80" s="27"/>
+      <c r="G80" s="26"/>
       <c r="H80" s="5"/>
       <c r="I80" s="5"/>
       <c r="J80" s="6"/>
@@ -3641,7 +3658,7 @@
       <c r="L80" s="5"/>
     </row>
     <row r="81" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G81" s="27"/>
+      <c r="G81" s="26"/>
       <c r="H81" s="5"/>
       <c r="I81" s="5"/>
       <c r="J81" s="6"/>
@@ -3649,7 +3666,7 @@
       <c r="L81" s="5"/>
     </row>
     <row r="82" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G82" s="27"/>
+      <c r="G82" s="26"/>
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
       <c r="J82" s="6"/>
@@ -3657,7 +3674,7 @@
       <c r="L82" s="5"/>
     </row>
     <row r="83" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G83" s="27"/>
+      <c r="G83" s="26"/>
       <c r="H83" s="5"/>
       <c r="I83" s="5"/>
       <c r="J83" s="6"/>
@@ -3665,7 +3682,7 @@
       <c r="L83" s="5"/>
     </row>
     <row r="84" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G84" s="27"/>
+      <c r="G84" s="26"/>
       <c r="H84" s="5"/>
       <c r="I84" s="5"/>
       <c r="J84" s="6"/>
@@ -3673,7 +3690,7 @@
       <c r="L84" s="5"/>
     </row>
     <row r="85" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G85" s="27"/>
+      <c r="G85" s="26"/>
       <c r="H85" s="5"/>
       <c r="I85" s="5"/>
       <c r="J85" s="6"/>
@@ -3681,7 +3698,7 @@
       <c r="L85" s="5"/>
     </row>
     <row r="86" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G86" s="27"/>
+      <c r="G86" s="26"/>
       <c r="H86" s="5"/>
       <c r="I86" s="5"/>
       <c r="J86" s="6"/>
@@ -3689,7 +3706,7 @@
       <c r="L86" s="5"/>
     </row>
     <row r="87" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G87" s="27"/>
+      <c r="G87" s="26"/>
       <c r="H87" s="5"/>
       <c r="I87" s="5"/>
       <c r="J87" s="6"/>
@@ -3697,7 +3714,7 @@
       <c r="L87" s="5"/>
     </row>
     <row r="88" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G88" s="27"/>
+      <c r="G88" s="26"/>
       <c r="H88" s="5"/>
       <c r="I88" s="5"/>
       <c r="J88" s="6"/>
@@ -3705,7 +3722,7 @@
       <c r="L88" s="5"/>
     </row>
     <row r="89" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G89" s="27"/>
+      <c r="G89" s="26"/>
       <c r="H89" s="5"/>
       <c r="I89" s="5"/>
       <c r="J89" s="6"/>
@@ -3713,7 +3730,7 @@
       <c r="L89" s="5"/>
     </row>
     <row r="90" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G90" s="27"/>
+      <c r="G90" s="26"/>
       <c r="H90" s="5"/>
       <c r="I90" s="5"/>
       <c r="J90" s="6"/>
@@ -3721,7 +3738,7 @@
       <c r="L90" s="5"/>
     </row>
     <row r="91" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G91" s="27"/>
+      <c r="G91" s="26"/>
       <c r="H91" s="5"/>
       <c r="I91" s="5"/>
       <c r="J91" s="6"/>
@@ -3729,7 +3746,7 @@
       <c r="L91" s="5"/>
     </row>
     <row r="92" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G92" s="27"/>
+      <c r="G92" s="26"/>
       <c r="H92" s="5"/>
       <c r="I92" s="5"/>
       <c r="J92" s="6"/>
@@ -3737,7 +3754,7 @@
       <c r="L92" s="5"/>
     </row>
     <row r="93" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G93" s="27"/>
+      <c r="G93" s="26"/>
       <c r="H93" s="5"/>
       <c r="I93" s="5"/>
       <c r="J93" s="6"/>
@@ -3745,7 +3762,7 @@
       <c r="L93" s="5"/>
     </row>
     <row r="94" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G94" s="27"/>
+      <c r="G94" s="26"/>
       <c r="H94" s="5"/>
       <c r="I94" s="5"/>
       <c r="J94" s="6"/>
@@ -3753,7 +3770,7 @@
       <c r="L94" s="5"/>
     </row>
     <row r="95" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G95" s="27"/>
+      <c r="G95" s="26"/>
       <c r="H95" s="5"/>
       <c r="I95" s="5"/>
       <c r="J95" s="6"/>
@@ -3761,7 +3778,7 @@
       <c r="L95" s="5"/>
     </row>
     <row r="96" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G96" s="27"/>
+      <c r="G96" s="26"/>
       <c r="H96" s="5"/>
       <c r="I96" s="5"/>
       <c r="J96" s="6"/>
@@ -3769,7 +3786,7 @@
       <c r="L96" s="5"/>
     </row>
     <row r="97" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G97" s="27"/>
+      <c r="G97" s="26"/>
       <c r="H97" s="5"/>
       <c r="I97" s="5"/>
       <c r="J97" s="6"/>
@@ -3777,7 +3794,7 @@
       <c r="L97" s="5"/>
     </row>
     <row r="98" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G98" s="27"/>
+      <c r="G98" s="26"/>
       <c r="H98" s="5"/>
       <c r="I98" s="5"/>
       <c r="J98" s="6"/>
@@ -3785,7 +3802,7 @@
       <c r="L98" s="5"/>
     </row>
     <row r="99" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G99" s="27"/>
+      <c r="G99" s="26"/>
       <c r="H99" s="5"/>
       <c r="I99" s="5"/>
       <c r="J99" s="6"/>
@@ -3793,7 +3810,7 @@
       <c r="L99" s="5"/>
     </row>
     <row r="100" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G100" s="27"/>
+      <c r="G100" s="26"/>
       <c r="H100" s="5"/>
       <c r="I100" s="5"/>
       <c r="J100" s="6"/>
@@ -3801,7 +3818,7 @@
       <c r="L100" s="5"/>
     </row>
     <row r="101" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G101" s="27"/>
+      <c r="G101" s="26"/>
       <c r="H101" s="5"/>
       <c r="I101" s="5"/>
       <c r="J101" s="6"/>
@@ -3809,7 +3826,7 @@
       <c r="L101" s="5"/>
     </row>
     <row r="102" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G102" s="27"/>
+      <c r="G102" s="26"/>
       <c r="H102" s="5"/>
       <c r="I102" s="5"/>
       <c r="J102" s="6"/>
@@ -3817,7 +3834,7 @@
       <c r="L102" s="5"/>
     </row>
     <row r="103" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G103" s="27"/>
+      <c r="G103" s="26"/>
       <c r="H103" s="5"/>
       <c r="I103" s="5"/>
       <c r="J103" s="6"/>
@@ -3825,7 +3842,7 @@
       <c r="L103" s="5"/>
     </row>
     <row r="104" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G104" s="27"/>
+      <c r="G104" s="26"/>
       <c r="H104" s="5"/>
       <c r="I104" s="5"/>
       <c r="J104" s="6"/>
@@ -3833,7 +3850,7 @@
       <c r="L104" s="5"/>
     </row>
     <row r="105" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G105" s="27"/>
+      <c r="G105" s="26"/>
       <c r="H105" s="5"/>
       <c r="I105" s="5"/>
       <c r="J105" s="6"/>
@@ -3841,7 +3858,7 @@
       <c r="L105" s="5"/>
     </row>
     <row r="106" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G106" s="27"/>
+      <c r="G106" s="26"/>
       <c r="H106" s="5"/>
       <c r="I106" s="5"/>
       <c r="J106" s="6"/>
@@ -3849,7 +3866,7 @@
       <c r="L106" s="5"/>
     </row>
     <row r="107" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G107" s="27"/>
+      <c r="G107" s="26"/>
       <c r="H107" s="5"/>
       <c r="I107" s="5"/>
       <c r="J107" s="6"/>
@@ -3857,7 +3874,7 @@
       <c r="L107" s="5"/>
     </row>
     <row r="108" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G108" s="27"/>
+      <c r="G108" s="26"/>
       <c r="H108" s="5"/>
       <c r="I108" s="5"/>
       <c r="J108" s="6"/>
@@ -3865,7 +3882,7 @@
       <c r="L108" s="5"/>
     </row>
     <row r="109" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G109" s="27"/>
+      <c r="G109" s="26"/>
       <c r="H109" s="5"/>
       <c r="I109" s="5"/>
       <c r="J109" s="6"/>
@@ -3873,7 +3890,7 @@
       <c r="L109" s="5"/>
     </row>
     <row r="110" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G110" s="27"/>
+      <c r="G110" s="26"/>
       <c r="H110" s="5"/>
       <c r="I110" s="5"/>
       <c r="J110" s="6"/>
@@ -3881,7 +3898,7 @@
       <c r="L110" s="5"/>
     </row>
     <row r="111" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G111" s="27"/>
+      <c r="G111" s="26"/>
       <c r="H111" s="5"/>
       <c r="I111" s="5"/>
       <c r="J111" s="6"/>
@@ -3889,7 +3906,7 @@
       <c r="L111" s="5"/>
     </row>
     <row r="112" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G112" s="27"/>
+      <c r="G112" s="26"/>
       <c r="H112" s="5"/>
       <c r="I112" s="5"/>
       <c r="J112" s="6"/>
@@ -3897,7 +3914,7 @@
       <c r="L112" s="5"/>
     </row>
     <row r="113" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G113" s="27"/>
+      <c r="G113" s="26"/>
       <c r="H113" s="5"/>
       <c r="I113" s="5"/>
       <c r="J113" s="6"/>
@@ -3905,7 +3922,7 @@
       <c r="L113" s="5"/>
     </row>
     <row r="114" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G114" s="27"/>
+      <c r="G114" s="26"/>
       <c r="H114" s="5"/>
       <c r="I114" s="5"/>
       <c r="J114" s="6"/>
@@ -3913,7 +3930,7 @@
       <c r="L114" s="5"/>
     </row>
     <row r="115" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G115" s="27"/>
+      <c r="G115" s="26"/>
       <c r="H115" s="5"/>
       <c r="I115" s="5"/>
       <c r="J115" s="6"/>
@@ -3921,7 +3938,7 @@
       <c r="L115" s="5"/>
     </row>
     <row r="116" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G116" s="27"/>
+      <c r="G116" s="26"/>
       <c r="H116" s="5"/>
       <c r="I116" s="5"/>
       <c r="J116" s="6"/>
@@ -3929,7 +3946,7 @@
       <c r="L116" s="5"/>
     </row>
     <row r="117" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G117" s="27"/>
+      <c r="G117" s="26"/>
       <c r="H117" s="5"/>
       <c r="I117" s="5"/>
       <c r="J117" s="6"/>
@@ -3937,7 +3954,7 @@
       <c r="L117" s="5"/>
     </row>
     <row r="118" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G118" s="27"/>
+      <c r="G118" s="26"/>
       <c r="H118" s="5"/>
       <c r="I118" s="5"/>
       <c r="J118" s="6"/>
@@ -3945,7 +3962,7 @@
       <c r="L118" s="5"/>
     </row>
     <row r="119" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G119" s="27"/>
+      <c r="G119" s="26"/>
       <c r="H119" s="5"/>
       <c r="I119" s="5"/>
       <c r="J119" s="6"/>
@@ -3953,7 +3970,7 @@
       <c r="L119" s="5"/>
     </row>
     <row r="120" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G120" s="27"/>
+      <c r="G120" s="26"/>
       <c r="H120" s="5"/>
       <c r="I120" s="5"/>
       <c r="J120" s="6"/>
@@ -3961,7 +3978,7 @@
       <c r="L120" s="5"/>
     </row>
     <row r="121" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G121" s="27"/>
+      <c r="G121" s="26"/>
       <c r="H121" s="5"/>
       <c r="I121" s="5"/>
       <c r="J121" s="6"/>
@@ -3969,7 +3986,7 @@
       <c r="L121" s="5"/>
     </row>
     <row r="122" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G122" s="27"/>
+      <c r="G122" s="26"/>
       <c r="H122" s="5"/>
       <c r="I122" s="5"/>
       <c r="J122" s="6"/>
@@ -3977,7 +3994,7 @@
       <c r="L122" s="5"/>
     </row>
     <row r="123" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G123" s="27"/>
+      <c r="G123" s="26"/>
       <c r="H123" s="5"/>
       <c r="I123" s="5"/>
       <c r="J123" s="6"/>
@@ -3985,7 +4002,7 @@
       <c r="L123" s="5"/>
     </row>
     <row r="124" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G124" s="27"/>
+      <c r="G124" s="26"/>
       <c r="H124" s="5"/>
       <c r="I124" s="5"/>
       <c r="J124" s="6"/>
@@ -3993,7 +4010,7 @@
       <c r="L124" s="5"/>
     </row>
     <row r="125" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G125" s="27"/>
+      <c r="G125" s="26"/>
       <c r="H125" s="5"/>
       <c r="I125" s="5"/>
       <c r="J125" s="6"/>
@@ -4001,7 +4018,7 @@
       <c r="L125" s="5"/>
     </row>
     <row r="126" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G126" s="27"/>
+      <c r="G126" s="26"/>
       <c r="H126" s="5"/>
       <c r="I126" s="5"/>
       <c r="J126" s="6"/>
@@ -4009,7 +4026,7 @@
       <c r="L126" s="5"/>
     </row>
     <row r="127" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G127" s="27"/>
+      <c r="G127" s="26"/>
       <c r="H127" s="5"/>
       <c r="I127" s="5"/>
       <c r="J127" s="6"/>
@@ -4017,7 +4034,7 @@
       <c r="L127" s="5"/>
     </row>
     <row r="128" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G128" s="27"/>
+      <c r="G128" s="26"/>
       <c r="H128" s="5"/>
       <c r="I128" s="5"/>
       <c r="J128" s="6"/>
@@ -4025,7 +4042,7 @@
       <c r="L128" s="5"/>
     </row>
     <row r="129" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G129" s="27"/>
+      <c r="G129" s="26"/>
       <c r="H129" s="5"/>
       <c r="I129" s="5"/>
       <c r="J129" s="6"/>
@@ -4033,7 +4050,7 @@
       <c r="L129" s="5"/>
     </row>
     <row r="130" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G130" s="27"/>
+      <c r="G130" s="26"/>
       <c r="H130" s="5"/>
       <c r="I130" s="5"/>
       <c r="J130" s="6"/>
@@ -4041,7 +4058,7 @@
       <c r="L130" s="5"/>
     </row>
     <row r="131" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G131" s="27"/>
+      <c r="G131" s="26"/>
       <c r="H131" s="5"/>
       <c r="I131" s="5"/>
       <c r="J131" s="6"/>
@@ -4049,7 +4066,7 @@
       <c r="L131" s="5"/>
     </row>
     <row r="132" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G132" s="27"/>
+      <c r="G132" s="26"/>
       <c r="H132" s="5"/>
       <c r="I132" s="5"/>
       <c r="J132" s="6"/>
@@ -4057,7 +4074,7 @@
       <c r="L132" s="5"/>
     </row>
     <row r="133" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G133" s="27"/>
+      <c r="G133" s="26"/>
       <c r="H133" s="5"/>
       <c r="I133" s="5"/>
       <c r="J133" s="6"/>
@@ -4065,7 +4082,7 @@
       <c r="L133" s="5"/>
     </row>
     <row r="134" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G134" s="27"/>
+      <c r="G134" s="26"/>
       <c r="H134" s="5"/>
       <c r="I134" s="5"/>
       <c r="J134" s="6"/>
@@ -4073,7 +4090,7 @@
       <c r="L134" s="5"/>
     </row>
     <row r="135" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G135" s="27"/>
+      <c r="G135" s="26"/>
       <c r="H135" s="5"/>
       <c r="I135" s="5"/>
       <c r="J135" s="6"/>
@@ -4081,7 +4098,7 @@
       <c r="L135" s="5"/>
     </row>
     <row r="136" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G136" s="27"/>
+      <c r="G136" s="26"/>
       <c r="H136" s="5"/>
       <c r="I136" s="5"/>
       <c r="J136" s="6"/>
@@ -4089,7 +4106,7 @@
       <c r="L136" s="5"/>
     </row>
     <row r="137" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G137" s="27"/>
+      <c r="G137" s="26"/>
       <c r="H137" s="5"/>
       <c r="I137" s="5"/>
       <c r="J137" s="6"/>
@@ -4097,7 +4114,7 @@
       <c r="L137" s="5"/>
     </row>
     <row r="138" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G138" s="27"/>
+      <c r="G138" s="26"/>
       <c r="H138" s="5"/>
       <c r="I138" s="5"/>
       <c r="J138" s="6"/>
@@ -4105,7 +4122,7 @@
       <c r="L138" s="5"/>
     </row>
     <row r="139" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G139" s="27"/>
+      <c r="G139" s="26"/>
       <c r="H139" s="5"/>
       <c r="I139" s="5"/>
       <c r="J139" s="6"/>
@@ -4113,7 +4130,7 @@
       <c r="L139" s="5"/>
     </row>
     <row r="140" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G140" s="27"/>
+      <c r="G140" s="26"/>
       <c r="H140" s="5"/>
       <c r="I140" s="5"/>
       <c r="J140" s="6"/>
@@ -4121,7 +4138,7 @@
       <c r="L140" s="5"/>
     </row>
     <row r="141" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G141" s="27"/>
+      <c r="G141" s="26"/>
       <c r="H141" s="5"/>
       <c r="I141" s="5"/>
       <c r="J141" s="6"/>
@@ -4129,7 +4146,7 @@
       <c r="L141" s="5"/>
     </row>
     <row r="142" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G142" s="27"/>
+      <c r="G142" s="26"/>
       <c r="H142" s="5"/>
       <c r="I142" s="5"/>
       <c r="J142" s="6"/>
@@ -4137,7 +4154,7 @@
       <c r="L142" s="5"/>
     </row>
     <row r="143" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G143" s="27"/>
+      <c r="G143" s="26"/>
       <c r="H143" s="5"/>
       <c r="I143" s="5"/>
       <c r="J143" s="6"/>
@@ -4145,7 +4162,7 @@
       <c r="L143" s="5"/>
     </row>
     <row r="144" spans="7:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G144" s="27"/>
+      <c r="G144" s="26"/>
       <c r="H144" s="5"/>
       <c r="I144" s="5"/>
       <c r="J144" s="6"/>

</xml_diff>